<commit_message>
HF - Authenticated user testcase commit helper, testcase, testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E4A138-25ED-4443-AF52-E8A73317F47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7E59C8-BCAF-4A9B-879F-33A18BB03A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="132">
   <si>
     <t>UserName</t>
   </si>
@@ -411,6 +411,18 @@
   </si>
   <si>
     <t>testingqaserdt</t>
+  </si>
+  <si>
+    <t>Lotuswave@123</t>
+  </si>
+  <si>
+    <t>headerlinks</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shop, Explore, Customize</t>
   </si>
 </sst>
 </file>
@@ -780,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BX33"/>
+  <dimension ref="A1:BY33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,81 +805,81 @@
     <col min="3" max="3" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="56.85546875" style="5"/>
-    <col min="29" max="29" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="16384" width="56.85546875" style="5"/>
+    <col min="6" max="7" width="30.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="56.85546875" style="5"/>
+    <col min="30" max="30" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -887,220 +899,227 @@
         <v>37</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="BW1" s="5" t="s">
+      <c r="BX1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BX1" s="5" t="s">
+      <c r="BY1" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -1112,31 +1131,33 @@
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="Q2" s="6"/>
+    </row>
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="9"/>
-    </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="Q3" s="6"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="9"/>
+    </row>
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>117</v>
       </c>
@@ -1149,11 +1170,11 @@
       <c r="F4" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6"/>
+      <c r="H4" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="7"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -1161,10 +1182,11 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="9"/>
-    </row>
-    <row r="5" spans="1:76" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q4" s="6"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="9"/>
+    </row>
+    <row r="5" spans="1:77" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>125</v>
       </c>
@@ -1177,16 +1199,17 @@
       <c r="F5" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="10"/>
-      <c r="AC5" s="9">
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="10"/>
+      <c r="AD5" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:76" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>126</v>
       </c>
@@ -1194,10 +1217,10 @@
       <c r="F6" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -1206,280 +1229,299 @@
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="AD8" s="5" t="s">
+      <c r="J8" s="6"/>
+      <c r="AE8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AE8" s="5" t="s">
+      <c r="AF8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AF8" s="5">
+      <c r="AG8" s="5">
         <v>123456</v>
       </c>
-      <c r="AG8" s="5" t="s">
+      <c r="AH8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AH8" s="5" t="s">
+      <c r="AI8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI8" s="5" t="s">
+      <c r="AJ8" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="5" t="s">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="AK9" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="AK10" s="2" t="s">
+    <row r="10" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AL10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AL10" s="2" t="s">
+      <c r="AM10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AM10" s="2" t="s">
+      <c r="AN10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AN10" s="2" t="s">
+      <c r="AO10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AO10" s="2" t="s">
+      <c r="AP10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AP10" s="2" t="s">
+      <c r="AQ10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AQ10" s="2">
+      <c r="AR10" s="2">
         <v>27</v>
       </c>
-      <c r="AR10" s="2" t="s">
+      <c r="AS10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AS10" s="2" t="s">
+      <c r="AT10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AT10" s="2" t="s">
+      <c r="AU10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AU10" s="2">
+      <c r="AV10" s="2">
         <v>2</v>
       </c>
-      <c r="AV10" s="2" t="s">
+      <c r="AW10" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="6"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="10"/>
-      <c r="AC13" s="9">
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="10"/>
+      <c r="AD13" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="AW14" s="5" t="s">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="AX14" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="AX15" s="5" t="s">
+    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="AY15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="AY15" s="5" t="s">
+      <c r="AZ15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="AZ15" s="5" t="s">
+      <c r="BA15" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BA15" s="6" t="s">
+      <c r="BB15" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="AX16" s="5" t="s">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="AY16" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="AY16" s="5" t="s">
+      <c r="AZ16" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="AZ16" s="6" t="s">
+      <c r="BA16" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="3:76" x14ac:dyDescent="0.25">
-      <c r="BA17" s="5" t="s">
+    <row r="17" spans="3:77" x14ac:dyDescent="0.25">
+      <c r="BB17" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="3:76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="6"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="10"/>
-      <c r="AC18" s="9">
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="10"/>
+      <c r="AD18" s="9">
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="3:76" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:77" x14ac:dyDescent="0.25">
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-      <c r="Y19" s="1"/>
-      <c r="AC19" s="5">
+      <c r="J19" s="6"/>
+      <c r="Z19" s="1"/>
+      <c r="AD19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="3:76" x14ac:dyDescent="0.25">
-      <c r="V20" s="8"/>
-      <c r="W20" s="9"/>
-    </row>
-    <row r="21" spans="3:76" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:77" x14ac:dyDescent="0.25">
+      <c r="W20" s="8"/>
+      <c r="X20" s="9"/>
+    </row>
+    <row r="21" spans="3:77" x14ac:dyDescent="0.25">
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="3:76" x14ac:dyDescent="0.25">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="3:77" x14ac:dyDescent="0.25">
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="V22" s="11"/>
-    </row>
-    <row r="24" spans="3:76" x14ac:dyDescent="0.25">
+      <c r="H22" s="6"/>
+      <c r="W22" s="11"/>
+    </row>
+    <row r="24" spans="3:77" x14ac:dyDescent="0.25">
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="BB24" s="5" t="s">
+      <c r="H24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="BC24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BC24" s="5" t="s">
+      <c r="BD24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BD24" s="5" t="s">
+      <c r="BE24" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="BE24" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="BF24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="BG24" s="5" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="BH24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BI24" s="5">
+      <c r="BI24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BJ24" s="5">
         <v>9</v>
       </c>
-      <c r="BJ24" s="5">
+      <c r="BK24" s="5">
         <v>10</v>
       </c>
-      <c r="BK24" s="5" t="s">
+      <c r="BL24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BL24" s="12">
+      <c r="BM24" s="12">
         <v>40000</v>
       </c>
-      <c r="BM24" s="5">
+      <c r="BN24" s="5">
         <v>12</v>
       </c>
-      <c r="BN24" s="12">
+      <c r="BO24" s="12">
         <v>1000000</v>
       </c>
-      <c r="BO24" s="5" t="s">
+      <c r="BP24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="BP24" s="5" t="s">
+      <c r="BQ24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="BQ24" s="5">
+      <c r="BR24" s="5">
         <v>57501</v>
       </c>
-      <c r="BR24" s="5" t="s">
+      <c r="BS24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="BS24" s="5" t="s">
+      <c r="BT24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="BT24" s="5" t="s">
+      <c r="BU24" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="BU24" s="5" t="s">
+      <c r="BV24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BV24" s="5" t="s">
+      <c r="BW24" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="3:76" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:77" x14ac:dyDescent="0.25">
       <c r="C25" s="6"/>
       <c r="E25" s="13"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-    </row>
-    <row r="27" spans="3:76" x14ac:dyDescent="0.25">
+      <c r="J25" s="6"/>
+    </row>
+    <row r="27" spans="3:77" x14ac:dyDescent="0.25">
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-    </row>
-    <row r="30" spans="3:76" x14ac:dyDescent="0.25">
-      <c r="BW30" s="5" t="s">
+      <c r="H27" s="6"/>
+    </row>
+    <row r="30" spans="3:77" x14ac:dyDescent="0.25">
+      <c r="BX30" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="3:76" x14ac:dyDescent="0.25">
-      <c r="BW31" s="5" t="s">
+    <row r="31" spans="3:77" x14ac:dyDescent="0.25">
+      <c r="BX31" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="3:76" x14ac:dyDescent="0.25">
-      <c r="BX32" s="5" t="s">
+    <row r="32" spans="3:77" x14ac:dyDescent="0.25">
+      <c r="BY32" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BA15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BB15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="F6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="F5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
     <hyperlink ref="C4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="B4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
+    <hyperlink ref="C2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
+    <hyperlink ref="B2" r:id="rId8" xr:uid="{66F73B81-B968-4C82-B793-9099BC4FF784}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mini cart functionality helper,testdata and main class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABAC6FD-3323-43E1-BC5D-83A188284C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C302C3-2054-4591-A0E7-DBE09A00DD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1320" windowWidth="15360" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
   <si>
     <t>UserName</t>
   </si>
@@ -486,6 +486,15 @@
   </si>
   <si>
     <t>United States,United States,France,Germany,UK,Australia,Hong Kong,Japan,Malaysia,New Zealand,Philippines,Singapore,South Korea,Colombia,Mexico,Uruguay</t>
+  </si>
+  <si>
+    <t>delete product</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Copper Brown</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -857,96 +866,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.7265625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="67.90625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="87.08984375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="30.7265625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="87.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="30.7109375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.7265625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="22.26953125" style="5" customWidth="1"/>
+    <col min="23" max="23" width="19.7109375" style="5" customWidth="1"/>
+    <col min="24" max="24" width="22.28515625" style="5" customWidth="1"/>
     <col min="25" max="25" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="56.81640625" style="5"/>
-    <col min="35" max="35" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="56.85546875" style="5"/>
+    <col min="35" max="35" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="16384" width="56.81640625" style="5"/>
+    <col min="80" max="80" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1192,7 +1201,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1239,7 +1248,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
@@ -1263,7 +1272,7 @@
       <c r="AB3" s="8"/>
       <c r="AC3" s="9"/>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>117</v>
       </c>
@@ -1292,7 +1301,7 @@
       <c r="AB4" s="8"/>
       <c r="AC4" s="9"/>
     </row>
-    <row r="5" spans="1:82" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:82" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>125</v>
       </c>
@@ -1315,7 +1324,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:82" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:82" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>126</v>
       </c>
@@ -1337,7 +1346,7 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>129</v>
       </c>
@@ -1353,7 +1362,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>132</v>
       </c>
@@ -1390,7 +1399,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>145</v>
       </c>
@@ -1401,7 +1410,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:82" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:82" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>147</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>149</v>
       </c>
@@ -1457,27 +1466,39 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="T12" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="H13" s="6"/>
+      <c r="T13" s="5">
+        <v>3</v>
+      </c>
       <c r="AE13" s="1"/>
       <c r="AF13" s="10"/>
       <c r="AI13" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
       <c r="BC14" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
       <c r="BD15" s="5" t="s">
         <v>107</v>
       </c>
@@ -1491,7 +1512,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
       <c r="BD16" s="5" t="s">
         <v>110</v>
       </c>
@@ -1502,12 +1523,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:82" x14ac:dyDescent="0.25">
       <c r="BG17" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="8:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H18" s="6"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="10"/>
@@ -1515,7 +1536,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:82" x14ac:dyDescent="0.25">
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -1526,22 +1547,22 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:82" x14ac:dyDescent="0.25">
       <c r="AB20" s="8"/>
       <c r="AC20" s="9"/>
     </row>
-    <row r="21" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:82" x14ac:dyDescent="0.25">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:82" x14ac:dyDescent="0.25">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="AB22" s="11"/>
     </row>
-    <row r="24" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:82" x14ac:dyDescent="0.25">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -1610,7 +1631,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="25" spans="8:82" x14ac:dyDescent="0.25">
       <c r="H25" s="6"/>
       <c r="J25" s="13"/>
       <c r="K25" s="6"/>
@@ -1619,27 +1640,27 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="27" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="27" spans="8:82" x14ac:dyDescent="0.25">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="30" spans="8:82" x14ac:dyDescent="0.25">
       <c r="CC30" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:82" x14ac:dyDescent="0.25">
       <c r="CC31" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="8:82" x14ac:dyDescent="0.35">
+    <row r="32" spans="8:82" x14ac:dyDescent="0.25">
       <c r="CD32" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>

</xml_diff>

<commit_message>
Cross-Sell carousel test case,helper and testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C302C3-2054-4591-A0E7-DBE09A00DD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DAD7D3-AFAF-4639-BD2E-33B7D7E803DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1320" windowWidth="15360" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="159">
   <si>
     <t>UserName</t>
   </si>
@@ -491,10 +491,19 @@
     <t>delete product</t>
   </si>
   <si>
-    <t>32 oz Wide Mouth - Copper Brown</t>
-  </si>
-  <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>crosssell</t>
+  </si>
+  <si>
+    <t>testproduct</t>
+  </si>
+  <si>
+    <t>S +$5.00</t>
+  </si>
+  <si>
+    <t>W32520</t>
   </si>
 </sst>
 </file>
@@ -866,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,10 +895,10 @@
     <col min="14" max="14" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19.7109375" style="5" customWidth="1"/>
@@ -1476,16 +1485,16 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="T12" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="T13" s="5">
-        <v>3</v>
+      <c r="U13" s="5">
+        <v>6</v>
       </c>
       <c r="AE13" s="1"/>
       <c r="AF13" s="10"/>
@@ -1494,6 +1503,18 @@
       </c>
     </row>
     <row r="14" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>157</v>
+      </c>
       <c r="BC14" s="5" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
added extenand fail log for hydroflask helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DAD7D3-AFAF-4639-BD2E-33B7D7E803DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA35D651-9124-4DBC-841A-5AD06A902CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="162">
   <si>
     <t>UserName</t>
   </si>
@@ -347,9 +347,6 @@
     <t>product</t>
   </si>
   <si>
-    <t>colorname</t>
-  </si>
-  <si>
     <t>USTG1001603054</t>
   </si>
   <si>
@@ -504,6 +501,18 @@
   </si>
   <si>
     <t>W32520</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Acai Purple</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>18 oz Standard Mouth</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
 </sst>
 </file>
@@ -873,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD33"/>
+  <dimension ref="A1:CE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,69 +908,70 @@
     <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.7109375" style="5" customWidth="1"/>
-    <col min="24" max="24" width="22.28515625" style="5" customWidth="1"/>
-    <col min="25" max="25" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="56.85546875" style="5"/>
-    <col min="35" max="35" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="16384" width="56.85546875" style="5"/>
+    <col min="23" max="23" width="19" style="5" customWidth="1"/>
+    <col min="24" max="24" width="19.7109375" style="5" customWidth="1"/>
+    <col min="25" max="25" width="22.28515625" style="5" customWidth="1"/>
+    <col min="26" max="26" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="56.85546875" style="5"/>
+    <col min="36" max="36" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" x14ac:dyDescent="0.25">
@@ -969,19 +979,19 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>0</v>
@@ -999,16 +1009,16 @@
         <v>37</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>22</v>
@@ -1032,182 +1042,182 @@
         <v>20</v>
       </c>
       <c r="W1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="CC1" s="5" t="s">
+      <c r="CD1" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="CD1" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:82" x14ac:dyDescent="0.25">
@@ -1215,19 +1225,19 @@
         <v>3</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -1236,40 +1246,41 @@
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>137</v>
       </c>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="6"/>
+      <c r="X2" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="AC2" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="AB2" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC2" s="5">
+      <c r="AD2" s="5">
         <v>9898989898</v>
       </c>
     </row>
     <row r="3" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -1278,25 +1289,26 @@
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="9"/>
+      <c r="W3" s="6"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="9"/>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N4" s="7"/>
       <c r="O4" s="6"/>
@@ -1307,43 +1319,44 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="9"/>
+      <c r="W4" s="6"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="9"/>
     </row>
     <row r="5" spans="1:82" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="K5" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="10"/>
-      <c r="AI5" s="9">
+        <v>121</v>
+      </c>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="10"/>
+      <c r="AJ5" s="9">
         <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:82" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H6" s="6"/>
       <c r="K6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -1354,15 +1367,16 @@
       <c r="T6" s="6"/>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
     </row>
     <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
@@ -1373,102 +1387,102 @@
     </row>
     <row r="8" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="AJ8" s="5" t="s">
+      <c r="AK8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AK8" s="5" t="s">
+      <c r="AL8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AL8" s="5">
+      <c r="AM8" s="5">
         <v>123456</v>
       </c>
-      <c r="AM8" s="5" t="s">
+      <c r="AN8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AN8" s="5" t="s">
+      <c r="AO8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AO8" s="5" t="s">
+      <c r="AP8" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="AP9" s="5" t="s">
+      <c r="AQ9" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:82" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AQ10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AR10" s="2" t="s">
+      <c r="AS10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AS10" s="2" t="s">
+      <c r="AT10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AT10" s="2" t="s">
+      <c r="AU10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU10" s="2" t="s">
+      <c r="AV10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AV10" s="2" t="s">
+      <c r="AW10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AW10" s="2">
+      <c r="AX10" s="2">
         <v>27</v>
       </c>
-      <c r="AX10" s="2" t="s">
+      <c r="AY10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AY10" s="2" t="s">
+      <c r="AZ10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AZ10" s="2" t="s">
+      <c r="BA10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BA10" s="2">
+      <c r="BB10" s="2">
         <v>2</v>
       </c>
-      <c r="BB10" s="2" t="s">
+      <c r="BC10" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
@@ -1477,7 +1491,7 @@
     </row>
     <row r="12" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1485,174 +1499,186 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="T12" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H13" s="6"/>
       <c r="U13" s="5">
         <v>6</v>
       </c>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="10"/>
-      <c r="AI13" s="9">
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="10"/>
+      <c r="AJ13" s="9">
         <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="T14" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="U14" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="BD14" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="T15" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="T14" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="BC14" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="BD15" s="5" t="s">
+      <c r="U15" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="W15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="BE15" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="BF15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BE15" s="5" t="s">
+      <c r="BG15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BF15" s="5" t="s">
+      <c r="BH15" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="BE16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BG15" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="BD16" s="5" t="s">
+      <c r="BF16" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="BE16" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="BF16" s="6" t="s">
+      <c r="BG16" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="8:82" x14ac:dyDescent="0.25">
-      <c r="BG17" s="5" t="s">
+    <row r="17" spans="8:83" x14ac:dyDescent="0.25">
+      <c r="BH17" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="8:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H18" s="6"/>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="10"/>
-      <c r="AI18" s="9">
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="10"/>
+      <c r="AJ18" s="9">
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="8:82" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:83" x14ac:dyDescent="0.25">
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
-      <c r="AE19" s="1"/>
-      <c r="AI19" s="5">
+      <c r="AF19" s="1"/>
+      <c r="AJ19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="8:82" x14ac:dyDescent="0.25">
-      <c r="AB20" s="8"/>
-      <c r="AC20" s="9"/>
-    </row>
-    <row r="21" spans="8:82" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:83" x14ac:dyDescent="0.25">
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="9"/>
+    </row>
+    <row r="21" spans="8:83" x14ac:dyDescent="0.25">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="8:82" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:83" x14ac:dyDescent="0.25">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="AB22" s="11"/>
-    </row>
-    <row r="24" spans="8:82" x14ac:dyDescent="0.25">
+      <c r="AC22" s="11"/>
+    </row>
+    <row r="24" spans="8:83" x14ac:dyDescent="0.25">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="T24" s="6"/>
-      <c r="BH24" s="5" t="s">
+      <c r="BI24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BI24" s="5" t="s">
+      <c r="BJ24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BJ24" s="5" t="s">
+      <c r="BK24" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="BK24" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="BL24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="BM24" s="5" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="BN24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BO24" s="5">
+      <c r="BO24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BP24" s="5">
         <v>9</v>
       </c>
-      <c r="BP24" s="5">
+      <c r="BQ24" s="5">
         <v>10</v>
       </c>
-      <c r="BQ24" s="5" t="s">
+      <c r="BR24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BR24" s="12">
+      <c r="BS24" s="12">
         <v>40000</v>
       </c>
-      <c r="BS24" s="5">
+      <c r="BT24" s="5">
         <v>12</v>
       </c>
-      <c r="BT24" s="12">
+      <c r="BU24" s="12">
         <v>1000000</v>
       </c>
-      <c r="BU24" s="5" t="s">
+      <c r="BV24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="BV24" s="5" t="s">
+      <c r="BW24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="BW24" s="5">
+      <c r="BX24" s="5">
         <v>57501</v>
       </c>
-      <c r="BX24" s="5" t="s">
+      <c r="BY24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="BY24" s="5" t="s">
+      <c r="BZ24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="BZ24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CB24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CC24" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="8:82" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:83" x14ac:dyDescent="0.25">
       <c r="H25" s="6"/>
       <c r="J25" s="13"/>
       <c r="K25" s="6"/>
@@ -1661,23 +1687,23 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="27" spans="8:82" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:83" x14ac:dyDescent="0.25">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="8:82" x14ac:dyDescent="0.25">
-      <c r="CC30" s="5" t="s">
+    <row r="30" spans="8:83" x14ac:dyDescent="0.25">
+      <c r="CD30" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="8:82" x14ac:dyDescent="0.25">
-      <c r="CC31" s="5" t="s">
+    <row r="31" spans="8:83" x14ac:dyDescent="0.25">
+      <c r="CD31" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="8:82" x14ac:dyDescent="0.25">
-      <c r="CD32" s="5" t="s">
+    <row r="32" spans="8:83" x14ac:dyDescent="0.25">
+      <c r="CE32" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1689,7 +1715,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BG15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BH15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="K6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="K5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>

</xml_diff>

<commit_message>
mini cart scroll and guest checkout place order
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA35D651-9124-4DBC-841A-5AD06A902CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC28813-36D4-4A8A-9707-11898B3936FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="173">
   <si>
     <t>UserName</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>cardNumber</t>
-  </si>
-  <si>
-    <t>ExpYear</t>
   </si>
   <si>
     <t>ExpMonth</t>
@@ -513,6 +510,42 @@
   </si>
   <si>
     <t>Color</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>PaymentDetails</t>
+  </si>
+  <si>
+    <t>ExpMonthYear</t>
+  </si>
+  <si>
+    <t>04/26</t>
+  </si>
+  <si>
+    <t>Shopproduct</t>
+  </si>
+  <si>
+    <t>4242424242424242</t>
+  </si>
+  <si>
+    <t>qa testing</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Everest Blue</t>
+  </si>
+  <si>
+    <t>Wide Flex Cap - Black</t>
+  </si>
+  <si>
+    <t>Wide Flex Cap - Pacific</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Copper Brown</t>
   </si>
 </sst>
 </file>
@@ -580,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -601,6 +634,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -882,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE33"/>
+  <dimension ref="A1:CD33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,90 +942,89 @@
     <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19" style="5" customWidth="1"/>
     <col min="24" max="24" width="19.7109375" style="5" customWidth="1"/>
     <col min="25" max="25" width="22.28515625" style="5" customWidth="1"/>
     <col min="26" max="26" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="56.85546875" style="5"/>
-    <col min="36" max="36" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="16384" width="56.85546875" style="5"/>
+    <col min="35" max="35" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>0</v>
@@ -1006,43 +1039,43 @@
         <v>5</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="S1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="W1" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>6</v>
@@ -1051,13 +1084,13 @@
         <v>7</v>
       </c>
       <c r="Z1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="AB1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC1" s="4" t="s">
         <v>8</v>
@@ -1072,44 +1105,46 @@
         <v>11</v>
       </c>
       <c r="AG1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>25</v>
+      <c r="AJ1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="AL1" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="AN1" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AO1" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AP1" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="AQ1" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AR1" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AS1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT1" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="AT1" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="AU1" s="4" t="s">
         <v>41</v>
@@ -1118,7 +1153,7 @@
         <v>42</v>
       </c>
       <c r="AW1" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="AX1" s="4" t="s">
         <v>49</v>
@@ -1130,16 +1165,16 @@
         <v>51</v>
       </c>
       <c r="BA1" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="BB1" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="BC1" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="BD1" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BE1" s="4" t="s">
         <v>65</v>
@@ -1148,10 +1183,10 @@
         <v>66</v>
       </c>
       <c r="BG1" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="BH1" s="4" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="BI1" s="4" t="s">
         <v>81</v>
@@ -1213,31 +1248,28 @@
       <c r="CB1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CC1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="CD1" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CC1" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -1246,41 +1278,46 @@
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>136</v>
       </c>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC2" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="AC2" s="11" t="s">
-        <v>139</v>
       </c>
       <c r="AD2" s="5">
         <v>9898989898</v>
       </c>
-    </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="14"/>
+    </row>
+    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -1293,22 +1330,22 @@
       <c r="AC3" s="8"/>
       <c r="AD3" s="9"/>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N4" s="7"/>
       <c r="O4" s="6"/>
@@ -1323,40 +1360,40 @@
       <c r="AC4" s="8"/>
       <c r="AD4" s="9"/>
     </row>
-    <row r="5" spans="1:82" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>123</v>
-      </c>
       <c r="K5" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="10"/>
-      <c r="AJ5" s="9">
+      <c r="AI5" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:82" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H6" s="6"/>
       <c r="K6" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -1369,14 +1406,14 @@
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
@@ -1385,81 +1422,84 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>151</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
+      <c r="AJ8" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="AK8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AM8" s="5">
+        <v>27</v>
+      </c>
+      <c r="AL8" s="5">
         <v>123456</v>
       </c>
+      <c r="AM8" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="AN8" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AO8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AP8" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="AP9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:81" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AQ9" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:82" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="B10" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+      <c r="AQ10" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="AR10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AS10" s="2" t="s">
+      <c r="AU10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AT10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AU10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AW10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX10" s="2">
+      <c r="AW10" s="2">
         <v>27</v>
+      </c>
+      <c r="AX10" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="AY10" s="2" t="s">
         <v>53</v>
@@ -1467,31 +1507,28 @@
       <c r="AZ10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BA10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="BB10" s="2">
+      <c r="BA10" s="2">
         <v>2</v>
       </c>
-      <c r="BC10" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="BB10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1499,12 +1536,12 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="T12" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H13" s="6"/>
       <c r="U13" s="5">
@@ -1512,39 +1549,42 @@
       </c>
       <c r="AF13" s="1"/>
       <c r="AG13" s="10"/>
-      <c r="AJ13" s="9">
+      <c r="AI13" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T14" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="U14" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="BC14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="T15" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="T14" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="BD14" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="U15" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="T15" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="U15" s="5" t="s">
-        <v>160</v>
-      </c>
       <c r="W15" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="BD15" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="BE15" s="5" t="s">
         <v>106</v>
@@ -1552,68 +1592,104 @@
       <c r="BF15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BG15" s="5" t="s">
+      <c r="BG15" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AF16" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="AG16" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="AI16" s="5">
+        <v>123</v>
+      </c>
+      <c r="BD16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BH15" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
       <c r="BE16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BF16" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="BG16" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="8:83" x14ac:dyDescent="0.25">
-      <c r="BH17" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="8:83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BF16" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="BG17" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="H18" s="6"/>
+      <c r="T18" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>169</v>
+      </c>
       <c r="AF18" s="3"/>
       <c r="AG18" s="10"/>
-      <c r="AJ18" s="9">
+      <c r="AI18" s="9">
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="8:83" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>168</v>
+      </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
+      <c r="T19" s="5" t="s">
+        <v>157</v>
+      </c>
       <c r="AF19" s="1"/>
-      <c r="AJ19" s="5">
+      <c r="AI19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="8:83" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:82" x14ac:dyDescent="0.25">
       <c r="AC20" s="8"/>
       <c r="AD20" s="9"/>
     </row>
-    <row r="21" spans="8:83" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:82" x14ac:dyDescent="0.25">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="8:83" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:82" x14ac:dyDescent="0.25">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="AC22" s="11"/>
     </row>
-    <row r="24" spans="8:83" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:82" x14ac:dyDescent="0.25">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="T24" s="6"/>
+      <c r="BH24" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="BI24" s="5" t="s">
         <v>71</v>
       </c>
@@ -1621,46 +1697,46 @@
         <v>72</v>
       </c>
       <c r="BK24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="BM24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BL24" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="BM24" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="BN24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BO24" s="5">
+        <v>9</v>
+      </c>
+      <c r="BP24" s="5">
+        <v>10</v>
+      </c>
+      <c r="BQ24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BO24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="BP24" s="5">
-        <v>9</v>
-      </c>
-      <c r="BQ24" s="5">
-        <v>10</v>
-      </c>
-      <c r="BR24" s="5" t="s">
+      <c r="BR24" s="12">
+        <v>40000</v>
+      </c>
+      <c r="BS24" s="5">
+        <v>12</v>
+      </c>
+      <c r="BT24" s="12">
+        <v>1000000</v>
+      </c>
+      <c r="BU24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="BV24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BS24" s="12">
-        <v>40000</v>
-      </c>
-      <c r="BT24" s="5">
-        <v>12</v>
-      </c>
-      <c r="BU24" s="12">
-        <v>1000000</v>
-      </c>
-      <c r="BV24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="BW24" s="5" t="s">
+      <c r="BW24" s="5">
+        <v>57501</v>
+      </c>
+      <c r="BX24" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="BX24" s="5">
-        <v>57501</v>
       </c>
       <c r="BY24" s="5" t="s">
         <v>77</v>
@@ -1669,16 +1745,13 @@
         <v>78</v>
       </c>
       <c r="CA24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="CB24" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="CB24" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="CC24" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="8:83" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:82" x14ac:dyDescent="0.25">
       <c r="H25" s="6"/>
       <c r="J25" s="13"/>
       <c r="K25" s="6"/>
@@ -1687,24 +1760,24 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="27" spans="8:83" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:82" x14ac:dyDescent="0.25">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="8:83" x14ac:dyDescent="0.25">
-      <c r="CD30" s="5" t="s">
+    <row r="30" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CC30" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CC31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="8:83" x14ac:dyDescent="0.25">
-      <c r="CD31" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="8:83" x14ac:dyDescent="0.25">
-      <c r="CE32" s="5" t="s">
-        <v>102</v>
+    <row r="32" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CD32" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="8:13" x14ac:dyDescent="0.25">
@@ -1715,7 +1788,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BH15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BG15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="K6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="K5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>

</xml_diff>

<commit_message>
OrderSummary DuringCheckout for both for hydroflask minicart scroll
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC28813-36D4-4A8A-9707-11898B3936FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358E5455-E9DB-46D8-8F08-81BAF534F188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="176">
   <si>
     <t>UserName</t>
   </si>
@@ -546,6 +546,15 @@
   </si>
   <si>
     <t>32 oz Wide Mouth - Copper Brown</t>
+  </si>
+  <si>
+    <t>Shipping method</t>
+  </si>
+  <si>
+    <t>methods</t>
+  </si>
+  <si>
+    <t>Federal Express - Ground</t>
   </si>
 </sst>
 </file>
@@ -916,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD33"/>
+  <dimension ref="A1:CE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,71 +952,72 @@
     <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19" style="5" customWidth="1"/>
-    <col min="24" max="24" width="19.7109375" style="5" customWidth="1"/>
-    <col min="25" max="25" width="22.28515625" style="5" customWidth="1"/>
-    <col min="26" max="26" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="16384" width="56.85546875" style="5"/>
+    <col min="22" max="22" width="30.5703125" style="5" customWidth="1"/>
+    <col min="23" max="23" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19" style="5" customWidth="1"/>
+    <col min="25" max="25" width="19.7109375" style="5" customWidth="1"/>
+    <col min="26" max="26" width="22.28515625" style="5" customWidth="1"/>
+    <col min="27" max="27" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1072,187 +1082,190 @@
         <v>18</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="W1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CC1" s="5" t="s">
+      <c r="CD1" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1287,25 +1300,26 @@
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="6"/>
+      <c r="Y2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AD2" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="AD2" s="5">
+      <c r="AE2" s="5">
         <v>9898989898</v>
       </c>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="14"/>
-    </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="14"/>
+    </row>
+    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
@@ -1327,10 +1341,11 @@
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="9"/>
-    </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="X3" s="6"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="9"/>
+    </row>
+    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
@@ -1357,10 +1372,11 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="9"/>
-    </row>
-    <row r="5" spans="1:81" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X4" s="6"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="9"/>
+    </row>
+    <row r="5" spans="1:82" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>123</v>
       </c>
@@ -1377,13 +1393,13 @@
       <c r="M5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="10"/>
-      <c r="AI5" s="9">
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="10"/>
+      <c r="AJ5" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:81" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:82" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>124</v>
       </c>
@@ -1405,8 +1421,9 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
-    </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="X6" s="6"/>
+    </row>
+    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>127</v>
       </c>
@@ -1422,7 +1439,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>130</v>
       </c>
@@ -1440,81 +1457,81 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="AJ8" s="5" t="s">
+      <c r="AK8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AK8" s="5" t="s">
+      <c r="AL8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AL8" s="5">
+      <c r="AM8" s="5">
         <v>123456</v>
       </c>
-      <c r="AM8" s="5" t="s">
+      <c r="AN8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AN8" s="5" t="s">
+      <c r="AO8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AO8" s="5" t="s">
+      <c r="AP8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>143</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="AP9" s="5" t="s">
+      <c r="AQ9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:81" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AQ10" s="2" t="s">
+      <c r="AR10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AR10" s="2" t="s">
+      <c r="AS10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AS10" s="2" t="s">
+      <c r="AT10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AT10" s="2" t="s">
+      <c r="AU10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AU10" s="2" t="s">
+      <c r="AV10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AV10" s="2" t="s">
+      <c r="AW10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW10" s="2">
+      <c r="AX10" s="2">
         <v>27</v>
       </c>
-      <c r="AX10" s="2" t="s">
+      <c r="AY10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AY10" s="2" t="s">
+      <c r="AZ10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AZ10" s="2" t="s">
+      <c r="BA10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BA10" s="2">
+      <c r="BB10" s="2">
         <v>2</v>
       </c>
-      <c r="BB10" s="2" t="s">
+      <c r="BC10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>147</v>
       </c>
@@ -1526,7 +1543,7 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>151</v>
       </c>
@@ -1539,7 +1556,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>152</v>
       </c>
@@ -1547,13 +1564,13 @@
       <c r="U13" s="5">
         <v>6</v>
       </c>
-      <c r="AF13" s="1"/>
-      <c r="AG13" s="10"/>
-      <c r="AI13" s="9">
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="10"/>
+      <c r="AJ13" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>153</v>
       </c>
@@ -1566,11 +1583,11 @@
       <c r="U14" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="BC14" s="5" t="s">
+      <c r="BD14" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>158</v>
       </c>
@@ -1580,46 +1597,46 @@
       <c r="U15" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="W15" s="5" t="s">
+      <c r="X15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="BD15" s="5" t="s">
+      <c r="BE15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BE15" s="5" t="s">
+      <c r="BF15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BF15" s="5" t="s">
+      <c r="BG15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BG15" s="6" t="s">
+      <c r="BH15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="AF16" s="11" t="s">
+      <c r="AG16" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="AG16" s="14" t="s">
+      <c r="AH16" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="AI16" s="5">
+      <c r="AJ16" s="5">
         <v>123</v>
       </c>
-      <c r="BD16" s="5" t="s">
+      <c r="BE16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BE16" s="5" t="s">
+      <c r="BF16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BF16" s="6" t="s">
+      <c r="BG16" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>165</v>
       </c>
@@ -1629,11 +1646,11 @@
       <c r="U17" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="BG17" s="5" t="s">
+      <c r="BH17" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>167</v>
       </c>
@@ -1644,13 +1661,13 @@
       <c r="U18" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="AF18" s="3"/>
-      <c r="AG18" s="10"/>
-      <c r="AI18" s="9">
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="10"/>
+      <c r="AJ18" s="9">
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>168</v>
       </c>
@@ -1662,96 +1679,102 @@
       <c r="T19" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="AF19" s="1"/>
-      <c r="AI19" s="5">
+      <c r="AG19" s="1"/>
+      <c r="AJ19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="AC20" s="8"/>
-      <c r="AD20" s="9"/>
-    </row>
-    <row r="21" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="V20" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="9"/>
+    </row>
+    <row r="21" spans="1:83" x14ac:dyDescent="0.25">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:83" x14ac:dyDescent="0.25">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="AC22" s="11"/>
-    </row>
-    <row r="24" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="AD22" s="11"/>
+    </row>
+    <row r="24" spans="1:83" x14ac:dyDescent="0.25">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="T24" s="6"/>
-      <c r="BH24" s="5" t="s">
+      <c r="BI24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BI24" s="5" t="s">
+      <c r="BJ24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BJ24" s="5" t="s">
+      <c r="BK24" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="BK24" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="BL24" s="5" t="s">
         <v>44</v>
       </c>
       <c r="BM24" s="5" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="BN24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BO24" s="5">
+      <c r="BO24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BP24" s="5">
         <v>9</v>
       </c>
-      <c r="BP24" s="5">
+      <c r="BQ24" s="5">
         <v>10</v>
       </c>
-      <c r="BQ24" s="5" t="s">
+      <c r="BR24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BR24" s="12">
+      <c r="BS24" s="12">
         <v>40000</v>
       </c>
-      <c r="BS24" s="5">
+      <c r="BT24" s="5">
         <v>12</v>
       </c>
-      <c r="BT24" s="12">
+      <c r="BU24" s="12">
         <v>1000000</v>
       </c>
-      <c r="BU24" s="5" t="s">
+      <c r="BV24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="BV24" s="5" t="s">
+      <c r="BW24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BW24" s="5">
+      <c r="BX24" s="5">
         <v>57501</v>
       </c>
-      <c r="BX24" s="5" t="s">
+      <c r="BY24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="BY24" s="5" t="s">
+      <c r="BZ24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="BZ24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CB24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CC24" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:83" x14ac:dyDescent="0.25">
       <c r="H25" s="6"/>
       <c r="J25" s="13"/>
       <c r="K25" s="6"/>
@@ -1760,23 +1783,23 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="27" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:83" x14ac:dyDescent="0.25">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="CC30" s="5" t="s">
+    <row r="30" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CD30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="CC31" s="5" t="s">
+    <row r="31" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CD31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="CD32" s="5" t="s">
+    <row r="32" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1788,7 +1811,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BG15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BH15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="K6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="K5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>

</xml_diff>

<commit_message>
Test cases Hydroflask add new address, no saved address, chatbot
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358E5455-E9DB-46D8-8F08-81BAF534F188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F9B6A2-F177-4023-AB39-D6CCBEB352EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="185">
   <si>
     <t>UserName</t>
   </si>
@@ -467,9 +467,6 @@
     <t>Chatoptions</t>
   </si>
   <si>
-    <t>OXOAnswers</t>
-  </si>
-  <si>
     <t>Subscription</t>
   </si>
   <si>
@@ -555,6 +552,36 @@
   </si>
   <si>
     <t>Federal Express - Ground</t>
+  </si>
+  <si>
+    <t>HydroAnswers</t>
+  </si>
+  <si>
+    <t>Discount Inquiries,Internal,Product Info</t>
+  </si>
+  <si>
+    <t>Newaddress</t>
+  </si>
+  <si>
+    <t>844 N colony road</t>
+  </si>
+  <si>
+    <t>Meriden</t>
+  </si>
+  <si>
+    <t>United State</t>
+  </si>
+  <si>
+    <t>06450</t>
+  </si>
+  <si>
+    <t>9898989898</t>
+  </si>
+  <si>
+    <t>Ground - Federal Express</t>
+  </si>
+  <si>
+    <t>Shippingmethods</t>
   </si>
 </sst>
 </file>
@@ -622,7 +649,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -644,6 +671,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -925,104 +954,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE33"/>
+  <dimension ref="A1:CF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="67.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="87.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="30.7109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.7265625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="52.26953125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="67.81640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="87.1796875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="30.7265625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.5703125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.54296875" style="5" customWidth="1"/>
     <col min="23" max="23" width="19" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19" style="5" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" style="5" customWidth="1"/>
-    <col min="26" max="26" width="22.28515625" style="5" customWidth="1"/>
+    <col min="25" max="25" width="19.7265625" style="5" customWidth="1"/>
+    <col min="26" max="26" width="22.26953125" style="5" customWidth="1"/>
     <col min="27" max="27" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="16384" width="56.85546875" style="5"/>
+    <col min="32" max="32" width="11" style="5" customWidth="1"/>
+    <col min="33" max="33" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="161.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="4.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="35.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="16384" width="56.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>143</v>
@@ -1082,13 +1112,13 @@
         <v>18</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>6</v>
@@ -1112,160 +1142,163 @@
         <v>9</v>
       </c>
       <c r="AF1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AG1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AH1" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="AI1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CD1" s="5" t="s">
+      <c r="CE1" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1308,7 +1341,7 @@
         <v>137</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AD2" s="11" t="s">
         <v>138</v>
@@ -1316,10 +1349,13 @@
       <c r="AE2" s="5">
         <v>9898989898</v>
       </c>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="14"/>
-    </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="AF2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="14"/>
+    </row>
+    <row r="3" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
@@ -1344,8 +1380,9 @@
       <c r="X3" s="6"/>
       <c r="AD3" s="8"/>
       <c r="AE3" s="9"/>
-    </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="AF3" s="9"/>
+    </row>
+    <row r="4" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
@@ -1375,8 +1412,9 @@
       <c r="X4" s="6"/>
       <c r="AD4" s="8"/>
       <c r="AE4" s="9"/>
-    </row>
-    <row r="5" spans="1:82" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF4" s="9"/>
+    </row>
+    <row r="5" spans="1:83" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>123</v>
       </c>
@@ -1393,13 +1431,13 @@
       <c r="M5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="10"/>
-      <c r="AJ5" s="9">
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="10"/>
+      <c r="AK5" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:82" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:83" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>124</v>
       </c>
@@ -1423,7 +1461,7 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>127</v>
       </c>
@@ -1439,7 +1477,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>130</v>
       </c>
@@ -1447,105 +1485,105 @@
         <v>142</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="AK8" s="5" t="s">
+      <c r="AL8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AL8" s="5" t="s">
+      <c r="AM8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AM8" s="5">
+      <c r="AN8" s="5">
         <v>123456</v>
       </c>
-      <c r="AN8" s="5" t="s">
+      <c r="AO8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AO8" s="5" t="s">
+      <c r="AP8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AP8" s="5" t="s">
+      <c r="AQ8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>143</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="AQ9" s="5" t="s">
+      <c r="AR9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:82" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:83" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AR10" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AS10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS10" s="2" t="s">
+      <c r="AT10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AT10" s="2" t="s">
+      <c r="AU10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AU10" s="2" t="s">
+      <c r="AV10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AV10" s="2" t="s">
+      <c r="AW10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AW10" s="2" t="s">
+      <c r="AX10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX10" s="2">
+      <c r="AY10" s="2">
         <v>27</v>
       </c>
-      <c r="AY10" s="2" t="s">
+      <c r="AZ10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ10" s="2" t="s">
+      <c r="BA10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BA10" s="2" t="s">
+      <c r="BB10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BB10" s="2">
+      <c r="BC10" s="2">
         <v>2</v>
       </c>
-      <c r="BC10" s="2" t="s">
+      <c r="BD10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1553,123 +1591,123 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="T12" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:83" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H13" s="6"/>
       <c r="U13" s="5">
         <v>6</v>
       </c>
-      <c r="AG13" s="1"/>
-      <c r="AH13" s="10"/>
-      <c r="AJ13" s="9">
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="10"/>
+      <c r="AK13" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="T14" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="U14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="BE14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:83" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="T15" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="T14" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="BD14" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="U15" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="T15" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="U15" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="X15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="BE15" s="5" t="s">
+      <c r="BF15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BF15" s="5" t="s">
+      <c r="BG15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BG15" s="5" t="s">
+      <c r="BH15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BH15" s="6" t="s">
+      <c r="BI15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="AG16" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH16" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="AI16" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK16" s="5">
+        <v>123</v>
+      </c>
+      <c r="BF16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="BG16" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="BH16" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="BI17" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="AH16" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="AJ16" s="5">
-        <v>123</v>
-      </c>
-      <c r="BE16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="BF16" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="BG16" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="T17" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="U17" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="BH17" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="H18" s="6"/>
       <c r="T18" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="10"/>
-      <c r="AJ18" s="9">
+        <v>168</v>
+      </c>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="10"/>
+      <c r="AK18" s="9">
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1677,104 +1715,139 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="T19" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="AG19" s="1"/>
-      <c r="AJ19" s="5">
+        <v>156</v>
+      </c>
+      <c r="AH19" s="1"/>
+      <c r="AK19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AD20" s="8"/>
       <c r="AE20" s="9"/>
-    </row>
-    <row r="21" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="AF20" s="9"/>
+    </row>
+    <row r="21" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-    </row>
-    <row r="22" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="Y21" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD21" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE21" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF21" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG21"/>
+    </row>
+    <row r="22" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="AD22" s="11"/>
     </row>
-    <row r="24" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="T24" s="6"/>
-      <c r="BI24" s="5" t="s">
+      <c r="BJ24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BJ24" s="5" t="s">
+      <c r="BK24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BK24" s="5" t="s">
+      <c r="BL24" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="BL24" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="BM24" s="5" t="s">
         <v>44</v>
       </c>
       <c r="BN24" s="5" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="BO24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BP24" s="5">
+      <c r="BP24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ24" s="5">
         <v>9</v>
       </c>
-      <c r="BQ24" s="5">
+      <c r="BR24" s="5">
         <v>10</v>
       </c>
-      <c r="BR24" s="5" t="s">
+      <c r="BS24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BS24" s="12">
+      <c r="BT24" s="12">
         <v>40000</v>
       </c>
-      <c r="BT24" s="5">
+      <c r="BU24" s="5">
         <v>12</v>
       </c>
-      <c r="BU24" s="12">
+      <c r="BV24" s="12">
         <v>1000000</v>
       </c>
-      <c r="BV24" s="5" t="s">
+      <c r="BW24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="BW24" s="5" t="s">
+      <c r="BX24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BX24" s="5">
+      <c r="BY24" s="5">
         <v>57501</v>
       </c>
-      <c r="BY24" s="5" t="s">
+      <c r="BZ24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="BZ24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CB24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CC24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="CC24" s="5" t="s">
+      <c r="CD24" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:84" x14ac:dyDescent="0.35">
       <c r="H25" s="6"/>
       <c r="J25" s="13"/>
       <c r="K25" s="6"/>
@@ -1783,27 +1856,27 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="27" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="CD30" s="5" t="s">
+    <row r="30" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="CE30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="CD31" s="5" t="s">
+    <row r="31" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="CE31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="CE32" s="5" t="s">
+    <row r="32" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="CF32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.35">
       <c r="H33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
@@ -1811,7 +1884,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BH15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BI15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="K6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="K5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>

</xml_diff>

<commit_message>
HF and OXO Test Cases Commit- Testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F9B6A2-F177-4023-AB39-D6CCBEB352EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D9F9B6A2-F177-4023-AB39-D6CCBEB352EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{319AAD00-CF2E-47A1-AFCC-539D753FAB0A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="192">
   <si>
     <t>UserName</t>
   </si>
@@ -582,6 +582,27 @@
   </si>
   <si>
     <t>Shippingmethods</t>
+  </si>
+  <si>
+    <t>ShippingAddress</t>
+  </si>
+  <si>
+    <t>lotus</t>
+  </si>
+  <si>
+    <t>wave</t>
+  </si>
+  <si>
+    <t>Grand Island</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>14072-2902</t>
   </si>
 </sst>
 </file>
@@ -956,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="Y7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AF21" sqref="AF21:AF22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,11 +1793,40 @@
       </c>
       <c r="AG21"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:84" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" t="s">
+        <v>186</v>
+      </c>
+      <c r="J22" t="s">
+        <v>187</v>
+      </c>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="AD22" s="11"/>
+      <c r="Y22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>191</v>
+      </c>
+      <c r="AE22">
+        <v>9898989898</v>
+      </c>
+      <c r="AF22" s="16" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="24" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K24" s="6"/>

</xml_diff>

<commit_message>
HF and OXO Account registration testcases commit - tetsdata, Tetscase, helper, XML files.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CA7A2FC1-B46F-464E-88B7-7BF27DAD65A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFF6910C-243C-4D36-8950-96841FEB5362}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{CA7A2FC1-B46F-464E-88B7-7BF27DAD65A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{888B2B73-E09F-4C09-9F0C-C3CEFD72A549}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="194">
   <si>
     <t>UserName</t>
   </si>
@@ -395,9 +395,6 @@
     <t>qatesting.lotuswave@gmail.com</t>
   </si>
   <si>
-    <t>awesrdtfgyuh</t>
-  </si>
-  <si>
     <t>invalidpassword</t>
   </si>
   <si>
@@ -600,6 +597,18 @@
   </si>
   <si>
     <t>W32410</t>
+  </si>
+  <si>
+    <t>Password2</t>
+  </si>
+  <si>
+    <t>awesr</t>
+  </si>
+  <si>
+    <t>rt65t</t>
+  </si>
+  <si>
+    <t>Rafeedha@123</t>
   </si>
 </sst>
 </file>
@@ -972,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CF33"/>
+  <dimension ref="A1:CG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -987,337 +996,341 @@
     <col min="5" max="5" width="67.81640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="87.1796875" style="5" customWidth="1"/>
     <col min="7" max="7" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="30.7265625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.54296875" style="5" customWidth="1"/>
-    <col min="23" max="23" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19" style="5" customWidth="1"/>
-    <col min="25" max="25" width="19.7265625" style="5" customWidth="1"/>
-    <col min="26" max="26" width="22.26953125" style="5" customWidth="1"/>
-    <col min="27" max="27" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11" style="5" customWidth="1"/>
-    <col min="33" max="33" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="56.81640625" style="5"/>
+    <col min="8" max="8" width="30.7265625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="30.7265625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.54296875" style="5" customWidth="1"/>
+    <col min="24" max="24" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" style="5" customWidth="1"/>
+    <col min="26" max="26" width="19.7265625" style="5" customWidth="1"/>
+    <col min="27" max="27" width="22.26953125" style="5" customWidth="1"/>
+    <col min="28" max="28" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11" style="5" customWidth="1"/>
+    <col min="34" max="34" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="161.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="4.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="35.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="6.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="16384" width="56.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>141</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="M1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="W1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="Y1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AF1" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="AG1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AI1" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="AJ1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CE1" s="5" t="s">
+      <c r="CF1" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1325,70 +1338,78 @@
         <v>121</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="6"/>
+      <c r="S2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="T2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE2" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="AC2" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD2" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE2" s="5">
+      <c r="AF2" s="5">
         <v>9898989898</v>
       </c>
-      <c r="AF2" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="14"/>
-    </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.35">
+      <c r="AG2" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="14"/>
+    </row>
+    <row r="3" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6"/>
+      <c r="O3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
@@ -1397,29 +1418,36 @@
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="9"/>
+      <c r="Y3" s="6"/>
+      <c r="AE3" s="8"/>
       <c r="AF3" s="9"/>
-    </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.35">
+      <c r="AG3" s="9"/>
+    </row>
+    <row r="4" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="5" t="s">
+      <c r="J4" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
@@ -1429,46 +1457,61 @@
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="9"/>
+      <c r="Y4" s="6"/>
+      <c r="AE4" s="8"/>
       <c r="AF4" s="9"/>
-    </row>
-    <row r="5" spans="1:83" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AG4" s="9"/>
+    </row>
+    <row r="5" spans="1:84" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>121</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K5" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="6"/>
+      <c r="N5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="10"/>
-      <c r="AK5" s="9">
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="10"/>
+      <c r="AL5" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:83" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="K6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="6"/>
+      <c r="N6" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -1479,472 +1522,474 @@
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
-    </row>
-    <row r="7" spans="1:83" x14ac:dyDescent="0.35">
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="M7" s="6"/>
+        <v>126</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
-    </row>
-    <row r="8" spans="1:83" x14ac:dyDescent="0.35">
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="AL8" s="5" t="s">
+      <c r="P8" s="6"/>
+      <c r="AM8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AM8" s="5" t="s">
+      <c r="AN8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AN8" s="5">
+      <c r="AO8" s="5">
         <v>123456</v>
       </c>
-      <c r="AO8" s="5" t="s">
+      <c r="AP8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AP8" s="5" t="s">
+      <c r="AQ8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AQ8" s="5" t="s">
+      <c r="AR8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="AS9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AR9" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:83" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AT10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AY10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ10" s="2">
+        <v>27</v>
+      </c>
+      <c r="BA10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD10" s="2">
+        <v>2</v>
+      </c>
+      <c r="BE10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="AS10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AU10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AY10" s="2">
-        <v>27</v>
-      </c>
-      <c r="AZ10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BB10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="BC10" s="2">
-        <v>2</v>
-      </c>
-      <c r="BD10" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="L11" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.35">
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K12" s="6"/>
+        <v>149</v>
+      </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-      <c r="T12" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:83" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P12" s="6"/>
+      <c r="U12" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="V13" s="5">
+        <v>6</v>
+      </c>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="10"/>
+      <c r="AL13" s="9">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="U13" s="5">
-        <v>6</v>
-      </c>
-      <c r="AH13" s="1"/>
-      <c r="AI13" s="10"/>
-      <c r="AK13" s="9">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q14" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="T14" s="5" t="s">
-        <v>154</v>
+      <c r="R14" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="U14" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="BE14" s="5" t="s">
+      <c r="V14" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="BF14" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="V15" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="T15" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="U15" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="X15" s="5" t="s">
+      <c r="Y15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="BF15" s="5" t="s">
+      <c r="BG15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BG15" s="5" t="s">
+      <c r="BH15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BH15" s="5" t="s">
+      <c r="BI15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BI15" s="6" t="s">
+      <c r="BJ15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="AH16" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="AI16" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI16" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ16" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL16" s="5">
+        <v>123</v>
+      </c>
+      <c r="BG16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="BH16" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="BI16" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="AK16" s="5">
-        <v>123</v>
-      </c>
-      <c r="BF16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="BG16" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="BH16" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="T17" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="U17" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="BI17" s="5" t="s">
+      <c r="V17" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="BJ17" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="U18" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="V18" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="10"/>
+      <c r="AL18" s="9">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="T18" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="AH18" s="3"/>
-      <c r="AI18" s="10"/>
-      <c r="AK18" s="9">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
-      <c r="T19" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH19" s="1"/>
-      <c r="AK19" s="5">
+      <c r="P19" s="6"/>
+      <c r="U19" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="AI19" s="1"/>
+      <c r="AL19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="V20" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="AD20" s="8"/>
-      <c r="AE20" s="9"/>
+        <v>169</v>
+      </c>
+      <c r="W20" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE20" s="8"/>
       <c r="AF20" s="9"/>
-    </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="AG20" s="9"/>
+    </row>
+    <row r="21" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="K21" s="6"/>
+      <c r="K21" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="Y21" t="s">
+      <c r="N21" s="6"/>
+      <c r="Z21" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA21" t="s">
         <v>175</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="AB21" t="s">
         <v>176</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AC21" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE21" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="AB21" t="s">
-        <v>158</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD21" s="15" t="s">
+      <c r="AF21" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="AE21" s="16" t="s">
+      <c r="AG21" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="AF21" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="AG21"/>
-    </row>
-    <row r="22" spans="1:84" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="AH21"/>
+    </row>
+    <row r="22" spans="1:85" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>181</v>
+      </c>
+      <c r="J22" t="s">
         <v>182</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>183</v>
       </c>
-      <c r="J22" t="s">
-        <v>184</v>
-      </c>
-      <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="Y22" t="s">
+      <c r="N22" s="6"/>
+      <c r="Z22" t="s">
         <v>35</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB22" t="s">
         <v>185</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AD22" t="s">
         <v>186</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AE22" t="s">
         <v>187</v>
       </c>
-      <c r="AD22" t="s">
-        <v>188</v>
-      </c>
-      <c r="AE22">
+      <c r="AF22">
         <v>9898989898</v>
       </c>
-      <c r="AF22" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="K24" s="6"/>
+      <c r="AG22" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:85" x14ac:dyDescent="0.35">
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="BJ24" s="5" t="s">
+      <c r="N24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="BK24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BK24" s="5" t="s">
+      <c r="BL24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BL24" s="5" t="s">
+      <c r="BM24" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="BM24" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="BN24" s="5" t="s">
         <v>44</v>
       </c>
       <c r="BO24" s="5" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="BP24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BQ24" s="5">
+      <c r="BQ24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR24" s="5">
         <v>9</v>
       </c>
-      <c r="BR24" s="5">
+      <c r="BS24" s="5">
         <v>10</v>
       </c>
-      <c r="BS24" s="5" t="s">
+      <c r="BT24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BT24" s="12">
+      <c r="BU24" s="12">
         <v>40000</v>
       </c>
-      <c r="BU24" s="5">
+      <c r="BV24" s="5">
         <v>12</v>
       </c>
-      <c r="BV24" s="12">
+      <c r="BW24" s="12">
         <v>1000000</v>
       </c>
-      <c r="BW24" s="5" t="s">
+      <c r="BX24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="BX24" s="5" t="s">
+      <c r="BY24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BY24" s="5">
+      <c r="BZ24" s="5">
         <v>57501</v>
       </c>
-      <c r="BZ24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CB24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CC24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CC24" s="5" t="s">
+      <c r="CD24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="CD24" s="5" t="s">
+      <c r="CE24" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="H25" s="6"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="6"/>
+    <row r="25" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="I25" s="6"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
-    </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="K27" s="6"/>
+      <c r="P25" s="6"/>
+    </row>
+    <row r="27" spans="1:85" x14ac:dyDescent="0.35">
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
-    </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="CE30" s="5" t="s">
+      <c r="N27" s="6"/>
+    </row>
+    <row r="30" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="CF30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="CE31" s="5" t="s">
+    <row r="31" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="CF31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="CF32" s="5" t="s">
+    <row r="32" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="CG32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.35">
-      <c r="H33" s="6"/>
-      <c r="K33" s="6"/>
+    <row r="33" spans="9:14" x14ac:dyDescent="0.35">
+      <c r="I33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BI15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BJ15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="K6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
-    <hyperlink ref="K5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
-    <hyperlink ref="H4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
+    <hyperlink ref="L6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="G4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
-    <hyperlink ref="H2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
+    <hyperlink ref="I2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
     <hyperlink ref="G2" r:id="rId8" xr:uid="{66F73B81-B968-4C82-B793-9099BC4FF784}"/>
-    <hyperlink ref="K2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
+    <hyperlink ref="L2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
     <hyperlink ref="D8" r:id="rId10" xr:uid="{5BE17100-3B6A-4B64-8895-3FBB3ED3E5B9}"/>
-    <hyperlink ref="K11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
+    <hyperlink ref="L11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
+    <hyperlink ref="H2" r:id="rId12" xr:uid="{14F9C943-C8EA-41B5-B2C0-1606A4BB7DAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Guest checkout shipping step for Hydroflask
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{CA7A2FC1-B46F-464E-88B7-7BF27DAD65A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{888B2B73-E09F-4C09-9F0C-C3CEFD72A549}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{CA7A2FC1-B46F-464E-88B7-7BF27DAD65A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25DCF9F2-0543-4617-AFE4-225203E43C60}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="199">
   <si>
     <t>UserName</t>
   </si>
@@ -609,6 +609,21 @@
   </si>
   <si>
     <t>Rafeedha@123</t>
+  </si>
+  <si>
+    <t>Invaliddiscountcode</t>
+  </si>
+  <si>
+    <t>validdiscountcode</t>
+  </si>
+  <si>
+    <t>Discount code</t>
+  </si>
+  <si>
+    <t>hydro30</t>
+  </si>
+  <si>
+    <t>GGQA$25</t>
   </si>
 </sst>
 </file>
@@ -981,102 +996,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CG33"/>
+  <dimension ref="A1:CH33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="CG1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CH23" sqref="CH23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="52.26953125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="67.81640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="87.1796875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7265625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="30.7265625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="52.21875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="67.77734375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="87.21875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.77734375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="30.77734375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="96.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="31.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.54296875" style="5" customWidth="1"/>
+    <col min="17" max="17" width="23.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.5546875" style="5" customWidth="1"/>
     <col min="24" max="24" width="19" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19" style="5" customWidth="1"/>
-    <col min="26" max="26" width="19.7265625" style="5" customWidth="1"/>
-    <col min="27" max="27" width="22.26953125" style="5" customWidth="1"/>
+    <col min="26" max="26" width="19.77734375" style="5" customWidth="1"/>
+    <col min="27" max="27" width="22.21875" style="5" customWidth="1"/>
     <col min="28" max="28" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="11" style="5" customWidth="1"/>
     <col min="34" max="34" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="29.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="161.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="4.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="35.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="146.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16.77734375" style="5" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="28.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="43.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.77734375" style="5" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="6.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="6.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="7.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="15.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="6.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="86" max="16384" width="56.81640625" style="5"/>
+    <col min="83" max="83" width="18.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="255.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="19.109375" style="5" customWidth="1"/>
+    <col min="86" max="16384" width="56.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1329,8 +1344,14 @@
       <c r="CF1" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="CG1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="CH1" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1390,7 +1411,7 @@
       <c r="AI2" s="11"/>
       <c r="AJ2" s="14"/>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
@@ -1423,7 +1444,7 @@
       <c r="AF3" s="9"/>
       <c r="AG3" s="9"/>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
@@ -1462,7 +1483,7 @@
       <c r="AF4" s="9"/>
       <c r="AG4" s="9"/>
     </row>
-    <row r="5" spans="1:84" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:86" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>122</v>
       </c>
@@ -1494,7 +1515,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:86" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>123</v>
       </c>
@@ -1524,7 +1545,7 @@
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>126</v>
       </c>
@@ -1540,7 +1561,7 @@
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>129</v>
       </c>
@@ -1577,7 +1598,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>142</v>
       </c>
@@ -1588,7 +1609,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:86" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>144</v>
       </c>
@@ -1632,7 +1653,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>145</v>
       </c>
@@ -1644,7 +1665,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>149</v>
       </c>
@@ -1657,7 +1678,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:86" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>150</v>
       </c>
@@ -1671,7 +1692,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>151</v>
       </c>
@@ -1688,7 +1709,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>154</v>
       </c>
@@ -1714,7 +1735,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>158</v>
       </c>
@@ -1737,7 +1758,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>161</v>
       </c>
@@ -1751,7 +1772,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:86" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>163</v>
       </c>
@@ -1768,7 +1789,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>164</v>
       </c>
@@ -1785,7 +1806,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
@@ -1796,7 +1817,7 @@
       <c r="AF20" s="9"/>
       <c r="AG20" s="9"/>
     </row>
-    <row r="21" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>173</v>
       </c>
@@ -1835,7 +1856,7 @@
       </c>
       <c r="AH21"/>
     </row>
-    <row r="22" spans="1:85" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:86" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>181</v>
       </c>
@@ -1870,7 +1891,18 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:86" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="CG23" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="CH23" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:86" x14ac:dyDescent="0.3">
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
@@ -1939,7 +1971,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:86" x14ac:dyDescent="0.3">
       <c r="I25" s="6"/>
       <c r="K25" s="13"/>
       <c r="L25" s="6"/>
@@ -1948,27 +1980,27 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="27" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:86" x14ac:dyDescent="0.3">
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
     </row>
-    <row r="30" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CF30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CF31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CG32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>

</xml_diff>

<commit_message>
change shipping address in address book oxo and HF
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{358E5455-E9DB-46D8-8F08-81BAF534F188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63BB08EB-FBAE-4A63-AF73-748BE8D171DE}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{3DA734F9-C539-4E6A-81E7-E3C9A4EE9EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70C76B7B-252F-4D4E-910C-7D8F6160EB0F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="208">
   <si>
     <t>UserName</t>
   </si>
@@ -395,9 +395,6 @@
     <t>qatesting.lotuswave@gmail.com</t>
   </si>
   <si>
-    <t>awesrdtfgyuh</t>
-  </si>
-  <si>
     <t>invalidpassword</t>
   </si>
   <si>
@@ -467,9 +464,6 @@
     <t>Chatoptions</t>
   </si>
   <si>
-    <t>OXOAnswers</t>
-  </si>
-  <si>
     <t>Subscription</t>
   </si>
   <si>
@@ -491,15 +485,9 @@
     <t>crosssell</t>
   </si>
   <si>
-    <t>testproduct</t>
-  </si>
-  <si>
     <t>S +$5.00</t>
   </si>
   <si>
-    <t>W32520</t>
-  </si>
-  <si>
     <t>32 oz Wide Mouth - Acai Purple</t>
   </si>
   <si>
@@ -557,19 +545,116 @@
     <t>Federal Express - Ground</t>
   </si>
   <si>
+    <t>HydroAnswers</t>
+  </si>
+  <si>
+    <t>Newaddress</t>
+  </si>
+  <si>
+    <t>844 N colony road</t>
+  </si>
+  <si>
+    <t>Meriden</t>
+  </si>
+  <si>
+    <t>United State</t>
+  </si>
+  <si>
+    <t>06450</t>
+  </si>
+  <si>
+    <t>9898989898</t>
+  </si>
+  <si>
+    <t>Ground - Federal Express</t>
+  </si>
+  <si>
+    <t>Shippingmethods</t>
+  </si>
+  <si>
+    <t>ShippingAddress</t>
+  </si>
+  <si>
+    <t>lotus</t>
+  </si>
+  <si>
+    <t>wave</t>
+  </si>
+  <si>
+    <t>Grand Island</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>14072-2902</t>
+  </si>
+  <si>
+    <t>Product Info,Warranty,Retail Information</t>
+  </si>
+  <si>
+    <t>W32410</t>
+  </si>
+  <si>
+    <t>Password2</t>
+  </si>
+  <si>
+    <t>awesr</t>
+  </si>
+  <si>
+    <t>rt65t</t>
+  </si>
+  <si>
+    <t>Rafeedha@123</t>
+  </si>
+  <si>
+    <t>New ShippingAddress</t>
+  </si>
+  <si>
+    <t>6 Walnut Valley Dr</t>
+  </si>
+  <si>
+    <t>Little Rock</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>72211</t>
+  </si>
+  <si>
+    <t>9999999999</t>
+  </si>
+  <si>
+    <t>Shipping address</t>
+  </si>
+  <si>
+    <t>testing QA
+6 Walnut Valley Dr
+Little Rock, Arkansas, 72211
+United States
+9999999999</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
     <t>Discount code</t>
   </si>
   <si>
+    <t>hydro30</t>
+  </si>
+  <si>
+    <t>GGQA$25</t>
+  </si>
+  <si>
     <t>Invaliddiscountcode</t>
   </si>
   <si>
     <t>validdiscountcode</t>
-  </si>
-  <si>
-    <t>hydro30</t>
-  </si>
-  <si>
-    <t>GGQA$25</t>
   </si>
 </sst>
 </file>
@@ -637,7 +722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -659,6 +744,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -940,354 +1030,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CG33"/>
+  <dimension ref="A1:CJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CE1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="CF21" sqref="CF21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="52.33203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="67.88671875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="87.109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="30.6640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="96.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.5546875" style="5" customWidth="1"/>
-    <col min="23" max="23" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19" style="5" customWidth="1"/>
-    <col min="25" max="25" width="19.6640625" style="5" customWidth="1"/>
-    <col min="26" max="26" width="22.33203125" style="5" customWidth="1"/>
-    <col min="27" max="27" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="29.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="161.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="21.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="4.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="23.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="35.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="146.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="28.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="43.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="6.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="12.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="13.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="15.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="15.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="18.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="255.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="16384" width="56.88671875" style="5"/>
+    <col min="1" max="1" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="87.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="30.7109375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.5703125" style="5" customWidth="1"/>
+    <col min="24" max="24" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" style="5" customWidth="1"/>
+    <col min="26" max="26" width="19.7109375" style="5" customWidth="1"/>
+    <col min="27" max="27" width="22.28515625" style="5" customWidth="1"/>
+    <col min="28" max="28" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11" style="5" customWidth="1"/>
+    <col min="34" max="34" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9" style="5" customWidth="1"/>
+    <col min="36" max="36" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="89" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>141</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="M1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="W1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="Y1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AH1" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AN1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AP1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CI1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="CE1" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="CF1" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="CG1" s="4"/>
-    </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1295,67 +1398,78 @@
         <v>121</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="6"/>
+      <c r="S2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="T2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE2" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="AC2" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="AD2" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE2" s="5">
+      <c r="AF2" s="5">
         <v>9898989898</v>
       </c>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="14"/>
-    </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.3">
+      <c r="AG2" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="14"/>
+    </row>
+    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6"/>
+      <c r="O3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
@@ -1364,28 +1478,36 @@
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="9"/>
-    </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.3">
+      <c r="Y3" s="6"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+    </row>
+    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="5" t="s">
+      <c r="J4" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
@@ -1395,45 +1517,63 @@
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="9"/>
-    </row>
-    <row r="5" spans="1:85" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y4" s="6"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+    </row>
+    <row r="5" spans="1:87" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>121</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K5" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="6"/>
+      <c r="N5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="10"/>
-      <c r="AJ5" s="9">
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="10"/>
+      <c r="AM5" s="9">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:85" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AN5" s="9"/>
+      <c r="AO5" s="9"/>
+    </row>
+    <row r="6" spans="1:87" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="K6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="6"/>
+      <c r="N6" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -1444,417 +1584,517 @@
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
-    </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.3">
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="M7" s="6"/>
+        <v>126</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
-    </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.3">
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="K8" s="6"/>
+        <v>148</v>
+      </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="AK8" s="5" t="s">
+      <c r="P8" s="6"/>
+      <c r="AP8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AL8" s="5" t="s">
+      <c r="AQ8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AM8" s="5">
+      <c r="AR8" s="5">
         <v>123456</v>
       </c>
-      <c r="AN8" s="5" t="s">
+      <c r="AS8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AO8" s="5" t="s">
+      <c r="AT8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AP8" s="5" t="s">
+      <c r="AU8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="AV9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:87" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AQ9" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AW10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BA10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BB10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC10" s="2">
+        <v>27</v>
+      </c>
+      <c r="BD10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BE10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BF10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BG10" s="2">
+        <v>2</v>
+      </c>
+      <c r="BH10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AR10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AW10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX10" s="2">
-        <v>27</v>
-      </c>
-      <c r="AY10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AZ10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BA10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="BB10" s="2">
-        <v>2</v>
-      </c>
-      <c r="BC10" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.3">
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K12" s="6"/>
+        <v>149</v>
+      </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-      <c r="T12" s="5" t="s">
+      <c r="P12" s="6"/>
+      <c r="U12" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="V13" s="5">
+        <v>6</v>
+      </c>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="10"/>
+      <c r="AM13" s="9">
+        <v>123</v>
+      </c>
+      <c r="AN13" s="9"/>
+      <c r="AO13" s="9"/>
+    </row>
+    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="V14" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="BI14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="13" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="U13" s="5">
-        <v>6</v>
-      </c>
-      <c r="AG13" s="1"/>
-      <c r="AH13" s="10"/>
-      <c r="AJ13" s="9">
+      <c r="U15" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="BJ15" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="BK15" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="BL15" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM15" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ16" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK16" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM16" s="5">
         <v>123</v>
       </c>
-    </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q14" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="T14" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="BD14" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="T15" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="U15" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="X15" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="BE15" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="BF15" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="BG15" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="BH15" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="AG16" s="11" t="s">
+      <c r="BJ16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="BK16" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="BL16" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="V17" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="AH16" s="14" t="s">
+      <c r="BM17" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="U18" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="V18" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="10"/>
+      <c r="AM18" s="9">
+        <v>1234</v>
+      </c>
+      <c r="AN18" s="9"/>
+      <c r="AO18" s="9"/>
+    </row>
+    <row r="19" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="AJ16" s="5">
-        <v>123</v>
-      </c>
-      <c r="BE16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="BF16" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="BG16" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="T17" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="U17" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="BH17" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="H18" s="6"/>
-      <c r="T18" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="10"/>
-      <c r="AJ18" s="9">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
-      <c r="T19" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="AG19" s="1"/>
-      <c r="AJ19" s="5">
+      <c r="P19" s="6"/>
+      <c r="U19" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="AJ19" s="1"/>
+      <c r="AM19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="W20" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+    </row>
+    <row r="21" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="V20" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="AD20" s="8"/>
-      <c r="AE20" s="9"/>
-    </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="K21" s="6"/>
+      <c r="J21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="CE21" s="5" t="s">
+      <c r="N21" s="6"/>
+      <c r="Z21" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE21" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF21" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="AG21" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="CF21" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="K22" s="6"/>
+      <c r="AH21"/>
+      <c r="AI21"/>
+    </row>
+    <row r="22" spans="1:88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>181</v>
+      </c>
+      <c r="J22" t="s">
+        <v>182</v>
+      </c>
+      <c r="K22" t="s">
+        <v>183</v>
+      </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="AD22" s="11"/>
-    </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="K24" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="Z22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF22">
+        <v>9898989898</v>
+      </c>
+      <c r="AG22" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:88" ht="180" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z23" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA23" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="AD23" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE23" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF23" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="AI23" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="BI24" s="5" t="s">
+      <c r="N24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="AN24" t="s">
+        <v>204</v>
+      </c>
+      <c r="AO24" t="s">
+        <v>205</v>
+      </c>
+      <c r="BN24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BJ24" s="5" t="s">
+      <c r="BO24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BK24" s="5" t="s">
+      <c r="BP24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BL24" s="5" t="s">
+      <c r="BQ24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BM24" s="5" t="s">
+      <c r="BR24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BN24" s="5" t="s">
+      <c r="BS24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BO24" s="5" t="s">
+      <c r="BT24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BP24" s="5">
+      <c r="BU24" s="5">
         <v>9</v>
       </c>
-      <c r="BQ24" s="5">
+      <c r="BV24" s="5">
         <v>10</v>
       </c>
-      <c r="BR24" s="5" t="s">
+      <c r="BW24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BS24" s="12">
+      <c r="BX24" s="12">
         <v>40000</v>
       </c>
-      <c r="BT24" s="5">
+      <c r="BY24" s="5">
         <v>12</v>
       </c>
-      <c r="BU24" s="12">
+      <c r="BZ24" s="12">
         <v>1000000</v>
       </c>
-      <c r="BV24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="BW24" s="5" t="s">
+      <c r="CB24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BX24" s="5">
+      <c r="CC24" s="5">
         <v>57501</v>
       </c>
-      <c r="BY24" s="5" t="s">
+      <c r="CD24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="BZ24" s="5" t="s">
+      <c r="CE24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CF24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CG24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="CC24" s="5" t="s">
+      <c r="CH24" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="H25" s="6"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="6"/>
+    <row r="25" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="I25" s="6"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
-    </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="K27" s="6"/>
+      <c r="P25" s="6"/>
+    </row>
+    <row r="27" spans="1:88" x14ac:dyDescent="0.25">
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
-    </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="CD30" s="5" t="s">
+      <c r="N27" s="6"/>
+    </row>
+    <row r="30" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="CI30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="CD31" s="5" t="s">
+    <row r="31" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="CI31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.3">
-      <c r="CE32" s="5" t="s">
+    <row r="32" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="CJ32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H33" s="6"/>
-      <c r="K33" s="6"/>
+    <row r="33" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BH15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BM15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="K6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
-    <hyperlink ref="K5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
-    <hyperlink ref="H4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
+    <hyperlink ref="L6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="G4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
-    <hyperlink ref="H2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
+    <hyperlink ref="I2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
     <hyperlink ref="G2" r:id="rId8" xr:uid="{66F73B81-B968-4C82-B793-9099BC4FF784}"/>
-    <hyperlink ref="K2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
+    <hyperlink ref="L2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
     <hyperlink ref="D8" r:id="rId10" xr:uid="{5BE17100-3B6A-4B64-8895-3FBB3ED3E5B9}"/>
-    <hyperlink ref="K11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
+    <hyperlink ref="L11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
+    <hyperlink ref="H2" r:id="rId12" xr:uid="{14F9C943-C8EA-41B5-B2C0-1606A4BB7DAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Account validation hydro,oxo test case ,helper test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{3DA734F9-C539-4E6A-81E7-E3C9A4EE9EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70C76B7B-252F-4D4E-910C-7D8F6160EB0F}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{3DA734F9-C539-4E6A-81E7-E3C9A4EE9EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEB86C76-17A7-4C74-BF2A-BC157BA06144}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="214">
   <si>
     <t>UserName</t>
   </si>
@@ -655,6 +655,24 @@
   </si>
   <si>
     <t>validdiscountcode</t>
+  </si>
+  <si>
+    <t>Adminusername</t>
+  </si>
+  <si>
+    <t>Adminpassword</t>
+  </si>
+  <si>
+    <t>AdminURL</t>
+  </si>
+  <si>
+    <t>mkoppanadam@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Amtlmcflmipq1!</t>
+  </si>
+  <si>
+    <t>https://na-preprod.hele.digital/heledigitaladmin</t>
   </si>
 </sst>
 </file>
@@ -722,7 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -749,6 +767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1030,487 +1049,503 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ33"/>
+  <dimension ref="A1:CM33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="67.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="87.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="30.7109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.5703125" style="5" customWidth="1"/>
-    <col min="24" max="24" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19" style="5" customWidth="1"/>
-    <col min="26" max="26" width="19.7109375" style="5" customWidth="1"/>
-    <col min="27" max="27" width="22.28515625" style="5" customWidth="1"/>
-    <col min="28" max="28" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11" style="5" customWidth="1"/>
-    <col min="34" max="34" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9" style="5" customWidth="1"/>
-    <col min="36" max="36" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="89" max="16384" width="56.85546875" style="5"/>
+    <col min="1" max="1" width="20.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.54296875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="52.26953125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="67.81640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="87.1796875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7265625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="30.7265625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="31.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.54296875" style="5" customWidth="1"/>
+    <col min="27" max="27" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19" style="5" customWidth="1"/>
+    <col min="29" max="29" width="19.7265625" style="5" customWidth="1"/>
+    <col min="30" max="30" width="22.26953125" style="5" customWidth="1"/>
+    <col min="31" max="31" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11" style="5" customWidth="1"/>
+    <col min="37" max="37" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9" style="5" customWidth="1"/>
+    <col min="39" max="39" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="161.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="4.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="20.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="35.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="6.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="92" max="16384" width="56.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CK1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CI1" s="5" t="s">
+      <c r="CL1" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="B2" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="AE2" s="11" t="s">
+      <c r="AH2" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="AF2" s="5">
+      <c r="AI2" s="5">
         <v>9898989898</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="14"/>
-    </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="14"/>
+    </row>
+    <row r="3" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="6"/>
+      <c r="M3" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-    </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+    </row>
+    <row r="4" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6" t="s">
+      <c r="K4" s="6"/>
+      <c r="L4" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="5" t="s">
+      <c r="P4" s="6"/>
+      <c r="Q4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
+      <c r="R4" s="7"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
@@ -1518,65 +1553,65 @@
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-    </row>
-    <row r="5" spans="1:87" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+    </row>
+    <row r="5" spans="1:90" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="5" t="s">
+      <c r="P5" s="6"/>
+      <c r="Q5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="10"/>
-      <c r="AM5" s="9">
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="10"/>
+      <c r="AP5" s="9">
         <v>123</v>
       </c>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
-    </row>
-    <row r="6" spans="1:87" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9"/>
+    </row>
+    <row r="6" spans="1:90" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5" t="s">
+      <c r="L6" s="6"/>
+      <c r="M6" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="M6" s="6"/>
-      <c r="N6" s="5" t="s">
+      <c r="P6" s="6"/>
+      <c r="Q6" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
@@ -1585,516 +1620,521 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+    </row>
+    <row r="7" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="I7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="6" t="s">
+      <c r="O7" s="6"/>
+      <c r="P7" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
-    </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+    </row>
+    <row r="8" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
-      <c r="AP8" s="5" t="s">
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="AS8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AQ8" s="5" t="s">
+      <c r="AT8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AR8" s="5">
+      <c r="AU8" s="5">
         <v>123456</v>
       </c>
-      <c r="AS8" s="5" t="s">
+      <c r="AV8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AT8" s="5" t="s">
+      <c r="AW8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AU8" s="5" t="s">
+      <c r="AX8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="AV9" s="5" t="s">
+      <c r="AY9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:87" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:90" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="AW10" s="2" t="s">
+      <c r="AZ10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AX10" s="2" t="s">
+      <c r="BA10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AY10" s="2" t="s">
+      <c r="BB10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AZ10" s="2" t="s">
+      <c r="BC10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="BA10" s="2" t="s">
+      <c r="BD10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BB10" s="2" t="s">
+      <c r="BE10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BC10" s="2">
+      <c r="BF10" s="2">
         <v>27</v>
       </c>
-      <c r="BD10" s="2" t="s">
+      <c r="BG10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BE10" s="2" t="s">
+      <c r="BH10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BF10" s="2" t="s">
+      <c r="BI10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BG10" s="2">
+      <c r="BJ10" s="2">
         <v>2</v>
       </c>
-      <c r="BH10" s="2" t="s">
+      <c r="BK10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="O11" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
       <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
-      <c r="U12" s="5" t="s">
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="X12" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:90" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="V13" s="5">
+      <c r="L13" s="6"/>
+      <c r="Y13" s="5">
         <v>6</v>
       </c>
-      <c r="AJ13" s="1"/>
-      <c r="AK13" s="10"/>
-      <c r="AM13" s="9">
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="10"/>
+      <c r="AP13" s="9">
         <v>123</v>
       </c>
-      <c r="AN13" s="9"/>
-      <c r="AO13" s="9"/>
-    </row>
-    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="AQ13" s="9"/>
+      <c r="AR13" s="9"/>
+    </row>
+    <row r="14" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="R14" s="5" t="s">
+      <c r="U14" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="X14" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="V14" s="5" t="s">
+      <c r="Y14" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="BI14" s="5" t="s">
+      <c r="BL14" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="U15" s="5" t="s">
+      <c r="X15" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="V15" s="5" t="s">
+      <c r="Y15" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="Y15" s="5" t="s">
+      <c r="AB15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="BJ15" s="5" t="s">
+      <c r="BM15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BK15" s="5" t="s">
+      <c r="BN15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BL15" s="5" t="s">
+      <c r="BO15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BM15" s="6" t="s">
+      <c r="BP15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="AJ16" s="11" t="s">
+      <c r="AM16" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AK16" s="14" t="s">
+      <c r="AN16" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="AM16" s="5">
+      <c r="AP16" s="5">
         <v>123</v>
       </c>
-      <c r="BJ16" s="5" t="s">
+      <c r="BM16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BK16" s="5" t="s">
+      <c r="BN16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BL16" s="6" t="s">
+      <c r="BO16" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="U17" s="5" t="s">
+      <c r="X17" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="V17" s="5" t="s">
+      <c r="Y17" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="BM17" s="5" t="s">
+      <c r="BP17" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:91" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="U18" s="5" t="s">
+      <c r="L18" s="6"/>
+      <c r="X18" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="V18" s="5" t="s">
+      <c r="Y18" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="AJ18" s="3"/>
-      <c r="AK18" s="10"/>
-      <c r="AM18" s="9">
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="10"/>
+      <c r="AP18" s="9">
         <v>1234</v>
       </c>
-      <c r="AN18" s="9"/>
-      <c r="AO18" s="9"/>
-    </row>
-    <row r="19" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="AQ18" s="9"/>
+      <c r="AR18" s="9"/>
+    </row>
+    <row r="19" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
-      <c r="U19" s="5" t="s">
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="X19" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="AJ19" s="1"/>
-      <c r="AM19" s="5">
+      <c r="AM19" s="1"/>
+      <c r="AP19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="W20" s="5" t="s">
+      <c r="Z20" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="AE20" s="8"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-    </row>
-    <row r="21" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
+    </row>
+    <row r="21" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="M21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="N21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="Z21" t="s">
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="AC21" t="s">
         <v>174</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AD21" t="s">
         <v>175</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AE21" t="s">
         <v>176</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="AF21" t="s">
         <v>157</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AG21" t="s">
         <v>157</v>
       </c>
-      <c r="AE21" s="15" t="s">
+      <c r="AH21" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="AF21" s="16" t="s">
+      <c r="AI21" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="AG21" s="16" t="s">
+      <c r="AJ21" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="AH21"/>
-      <c r="AI21"/>
-    </row>
-    <row r="22" spans="1:88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK21"/>
+      <c r="AL21"/>
+    </row>
+    <row r="22" spans="1:91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>181</v>
       </c>
-      <c r="J22" t="s">
+      <c r="M22" t="s">
         <v>182</v>
       </c>
-      <c r="K22" t="s">
+      <c r="N22" t="s">
         <v>183</v>
       </c>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="Z22" t="s">
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="AC22" t="s">
         <v>35</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AD22" t="s">
         <v>184</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AE22" t="s">
         <v>185</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AG22" t="s">
         <v>186</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AH22" t="s">
         <v>187</v>
       </c>
-      <c r="AF22">
+      <c r="AI22">
         <v>9898989898</v>
       </c>
-      <c r="AG22" s="16" t="s">
+      <c r="AJ22" s="16" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:88" ht="180" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:91" ht="174" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="M23" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="N23" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="Z23" s="5" t="s">
+      <c r="AC23" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="AA23" s="5" t="s">
+      <c r="AD23" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="AD23" s="5" t="s">
+      <c r="AG23" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="AE23" s="11" t="s">
+      <c r="AH23" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="AF23" s="11" t="s">
+      <c r="AI23" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="AI23" s="17" t="s">
+      <c r="AL23" s="17" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="AN24" t="s">
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="AQ24" t="s">
         <v>204</v>
       </c>
-      <c r="AO24" t="s">
+      <c r="AR24" t="s">
         <v>205</v>
       </c>
-      <c r="BN24" s="5" t="s">
+      <c r="BQ24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BO24" s="5" t="s">
+      <c r="BR24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BP24" s="5" t="s">
+      <c r="BS24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BQ24" s="5" t="s">
+      <c r="BT24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BR24" s="5" t="s">
+      <c r="BU24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BS24" s="5" t="s">
+      <c r="BV24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BT24" s="5" t="s">
+      <c r="BW24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BU24" s="5">
+      <c r="BX24" s="5">
         <v>9</v>
       </c>
-      <c r="BV24" s="5">
+      <c r="BY24" s="5">
         <v>10</v>
       </c>
-      <c r="BW24" s="5" t="s">
+      <c r="BZ24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BX24" s="12">
+      <c r="CA24" s="12">
         <v>40000</v>
       </c>
-      <c r="BY24" s="5">
+      <c r="CB24" s="5">
         <v>12</v>
       </c>
-      <c r="BZ24" s="12">
+      <c r="CC24" s="12">
         <v>1000000</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CD24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CE24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="CC24" s="5">
+      <c r="CF24" s="5">
         <v>57501</v>
       </c>
-      <c r="CD24" s="5" t="s">
+      <c r="CG24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="CE24" s="5" t="s">
+      <c r="CH24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CF24" s="5" t="s">
+      <c r="CI24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CG24" s="5" t="s">
+      <c r="CJ24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="CH24" s="5" t="s">
+      <c r="CK24" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="I25" s="6"/>
-      <c r="K25" s="13"/>
+    <row r="25" spans="1:91" x14ac:dyDescent="0.35">
       <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
+      <c r="N25" s="13"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
-    </row>
-    <row r="27" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-    </row>
-    <row r="30" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="CI30" s="5" t="s">
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+    </row>
+    <row r="27" spans="1:91" x14ac:dyDescent="0.35">
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+    </row>
+    <row r="30" spans="1:91" x14ac:dyDescent="0.35">
+      <c r="CL30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="CI31" s="5" t="s">
+    <row r="31" spans="1:91" x14ac:dyDescent="0.35">
+      <c r="CL31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="CJ32" s="5" t="s">
+    <row r="32" spans="1:91" x14ac:dyDescent="0.35">
+      <c r="CM32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I33" s="6"/>
+    <row r="33" spans="12:17" x14ac:dyDescent="0.35">
       <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BM15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="L6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
-    <hyperlink ref="L5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
-    <hyperlink ref="I4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
-    <hyperlink ref="I2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
-    <hyperlink ref="G2" r:id="rId8" xr:uid="{66F73B81-B968-4C82-B793-9099BC4FF784}"/>
-    <hyperlink ref="L2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
-    <hyperlink ref="D8" r:id="rId10" xr:uid="{5BE17100-3B6A-4B64-8895-3FBB3ED3E5B9}"/>
-    <hyperlink ref="L11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
-    <hyperlink ref="H2" r:id="rId12" xr:uid="{14F9C943-C8EA-41B5-B2C0-1606A4BB7DAF}"/>
+    <hyperlink ref="BP15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
+    <hyperlink ref="O6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
+    <hyperlink ref="O5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
+    <hyperlink ref="L4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
+    <hyperlink ref="J4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
+    <hyperlink ref="L2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
+    <hyperlink ref="J2" r:id="rId8" xr:uid="{66F73B81-B968-4C82-B793-9099BC4FF784}"/>
+    <hyperlink ref="O2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
+    <hyperlink ref="G8" r:id="rId10" xr:uid="{5BE17100-3B6A-4B64-8895-3FBB3ED3E5B9}"/>
+    <hyperlink ref="O11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
+    <hyperlink ref="K2" r:id="rId12" xr:uid="{14F9C943-C8EA-41B5-B2C0-1606A4BB7DAF}"/>
+    <hyperlink ref="B2" r:id="rId13" xr:uid="{1F6FEAF9-8E7E-47DB-A889-AED537C581F6}"/>
+    <hyperlink ref="D2" r:id="rId14" xr:uid="{361190E9-97EB-4336-8DE0-98559A3DB48A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HF clossadd for all test cases,helper,testdata and smoke xmls for oxo,hf
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{3DA734F9-C539-4E6A-81E7-E3C9A4EE9EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEB86C76-17A7-4C74-BF2A-BC157BA06144}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{3DA734F9-C539-4E6A-81E7-E3C9A4EE9EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87E218E3-78AE-411B-B058-0D45A24ACDA8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="219">
   <si>
     <t>UserName</t>
   </si>
@@ -673,6 +673,25 @@
   </si>
   <si>
     <t>https://na-preprod.hele.digital/heledigitaladmin</t>
+  </si>
+  <si>
+    <t>New BillingAddress</t>
+  </si>
+  <si>
+    <t>715 christiana Ave</t>
+  </si>
+  <si>
+    <t>Wilmington</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>TEST TEST
+715 christiana Ave
+Wilmington, Delaware, 19801
+United States
+9898989898</t>
   </si>
 </sst>
 </file>
@@ -760,7 +779,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -768,6 +786,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1051,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CM33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1151,13 +1170,13 @@
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>210</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -1486,7 +1505,7 @@
         <v>179</v>
       </c>
       <c r="AM2" s="11"/>
-      <c r="AN2" s="14"/>
+      <c r="AN2" s="13"/>
     </row>
     <row r="3" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
@@ -1823,7 +1842,7 @@
       <c r="AM16" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AN16" s="14" t="s">
+      <c r="AN16" s="13" t="s">
         <v>160</v>
       </c>
       <c r="AP16" s="5">
@@ -1928,13 +1947,13 @@
       <c r="AG21" t="s">
         <v>157</v>
       </c>
-      <c r="AH21" s="15" t="s">
+      <c r="AH21" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="AI21" s="16" t="s">
+      <c r="AI21" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="AJ21" s="16" t="s">
+      <c r="AJ21" s="15" t="s">
         <v>179</v>
       </c>
       <c r="AK21"/>
@@ -1971,7 +1990,7 @@
       <c r="AI22">
         <v>9898989898</v>
       </c>
-      <c r="AJ22" s="16" t="s">
+      <c r="AJ22" s="15" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2000,7 +2019,7 @@
       <c r="AI23" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="AL23" s="17" t="s">
+      <c r="AL23" s="16" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2082,14 +2101,44 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:91" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="L25" s="6"/>
-      <c r="N25" s="13"/>
+      <c r="M25" t="s">
+        <v>131</v>
+      </c>
+      <c r="N25" s="18" t="s">
+        <v>131</v>
+      </c>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
+      <c r="AC25" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>216</v>
+      </c>
+      <c r="AE25"/>
+      <c r="AF25"/>
+      <c r="AG25" t="s">
+        <v>217</v>
+      </c>
+      <c r="AH25">
+        <v>19801</v>
+      </c>
+      <c r="AI25">
+        <v>9898989898</v>
+      </c>
+      <c r="AJ25"/>
+      <c r="AK25"/>
+      <c r="AL25" s="16" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="27" spans="1:91" x14ac:dyDescent="0.35">
       <c r="O27" s="6"/>

</xml_diff>

<commit_message>
HF prodeal testcase commit - tetscase, helper, testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{3DA734F9-C539-4E6A-81E7-E3C9A4EE9EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87E218E3-78AE-411B-B058-0D45A24ACDA8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA975B7-1201-40C9-A1A8-CE8CC1B070C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="229">
   <si>
     <t>UserName</t>
   </si>
@@ -693,6 +693,36 @@
 United States
 9898989898</t>
   </si>
+  <si>
+    <t>Prodeal access code</t>
+  </si>
+  <si>
+    <t>Prodeal invalid access code</t>
+  </si>
+  <si>
+    <t>prodealaccesscode</t>
+  </si>
+  <si>
+    <t>GGQA12</t>
+  </si>
+  <si>
+    <t>FSRE21</t>
+  </si>
+  <si>
+    <t>lotuswave</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>CompanyEmail</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>pro deal form</t>
+  </si>
 </sst>
 </file>
 
@@ -701,7 +731,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,6 +761,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -759,7 +802,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -787,6 +830,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1068,105 +1114,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CM33"/>
+  <dimension ref="A1:CR33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="20.7265625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.54296875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="52.26953125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="67.81640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="87.1796875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7265625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="30.7265625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="31.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.54296875" style="5" customWidth="1"/>
-    <col min="27" max="27" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19" style="5" customWidth="1"/>
-    <col min="29" max="29" width="19.7265625" style="5" customWidth="1"/>
-    <col min="30" max="30" width="22.26953125" style="5" customWidth="1"/>
-    <col min="31" max="31" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11" style="5" customWidth="1"/>
-    <col min="37" max="37" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9" style="5" customWidth="1"/>
-    <col min="39" max="39" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="17.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="92" max="16384" width="56.81640625" style="5"/>
+    <col min="1" max="1" width="26" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="43.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.7109375" style="5" customWidth="1"/>
+    <col min="11" max="12" width="52.28515625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="67.85546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="87.140625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="5" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="30.7109375" style="5" customWidth="1"/>
+    <col min="22" max="22" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="38" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="29.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.5703125" style="5" customWidth="1"/>
+    <col min="32" max="32" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19" style="5" customWidth="1"/>
+    <col min="34" max="34" width="19.7109375" style="5" customWidth="1"/>
+    <col min="35" max="35" width="22.28515625" style="5" customWidth="1"/>
+    <col min="36" max="36" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11" style="5" customWidth="1"/>
+    <col min="42" max="42" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9" style="5" customWidth="1"/>
+    <col min="44" max="44" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="97" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1185,260 +1234,275 @@
       <c r="F1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CK1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CL1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CN1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CO1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CP1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CL1" s="5" t="s">
+      <c r="CQ1" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1451,739 +1515,765 @@
       <c r="D2" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="G2" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="I2" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="O2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
       <c r="U2" s="6"/>
-      <c r="V2" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>134</v>
-      </c>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="5" t="s">
+      <c r="AA2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="AH2" s="11" t="s">
+      <c r="AM2" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="AI2" s="5">
+      <c r="AN2" s="5">
         <v>9898989898</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AO2" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="13"/>
-    </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="AR2" s="11"/>
+      <c r="AS2" s="13"/>
+    </row>
+    <row r="3" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="5" t="s">
+      <c r="Q3" s="6"/>
+      <c r="R3" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
+      <c r="W3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="9"/>
-    </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="9"/>
+      <c r="AO3" s="9"/>
+    </row>
+    <row r="4" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6" t="s">
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="S4" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="T4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="5" t="s">
+      <c r="U4" s="6"/>
+      <c r="V4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="R4" s="7"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
+      <c r="W4" s="7"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-    </row>
-    <row r="5" spans="1:90" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="9"/>
+      <c r="AO4" s="9"/>
+    </row>
+    <row r="5" spans="1:95" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>131</v>
-      </c>
       <c r="O5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="5" t="s">
+      <c r="P5" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="V5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AM5" s="1"/>
-      <c r="AN5" s="10"/>
-      <c r="AP5" s="9">
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="10"/>
+      <c r="AU5" s="9">
         <v>123</v>
       </c>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-    </row>
-    <row r="6" spans="1:90" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AV5" s="9"/>
+      <c r="AW5" s="9"/>
+    </row>
+    <row r="6" spans="1:95" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="5" t="s">
+      <c r="Q6" s="6"/>
+      <c r="R6" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="S6" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="T6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="5" t="s">
+      <c r="U6" s="6"/>
+      <c r="V6" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
-    </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+    </row>
+    <row r="7" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6" t="s">
+      <c r="Q7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
       <c r="V7" s="6"/>
-    </row>
-    <row r="8" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+    </row>
+    <row r="8" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="L8" s="6"/>
+      <c r="M8" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="N8" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="AS8" s="5" t="s">
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="AX8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AT8" s="5" t="s">
+      <c r="AY8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AU8" s="5">
+      <c r="AZ8" s="5">
         <v>123456</v>
       </c>
-      <c r="AV8" s="5" t="s">
+      <c r="BA8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AW8" s="5" t="s">
+      <c r="BB8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AX8" s="5" t="s">
+      <c r="BC8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>142</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="AY9" s="5" t="s">
+      <c r="BD9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:90" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="AZ10" s="2" t="s">
+      <c r="BE10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="BA10" s="2" t="s">
+      <c r="BF10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BB10" s="2" t="s">
+      <c r="BG10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BC10" s="2" t="s">
+      <c r="BH10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="BD10" s="2" t="s">
+      <c r="BI10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BE10" s="2" t="s">
+      <c r="BJ10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BF10" s="2">
+      <c r="BK10" s="2">
         <v>27</v>
       </c>
-      <c r="BG10" s="2" t="s">
+      <c r="BL10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BH10" s="2" t="s">
+      <c r="BM10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BI10" s="2" t="s">
+      <c r="BN10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BJ10" s="2">
+      <c r="BO10" s="2">
         <v>2</v>
       </c>
-      <c r="BK10" s="2" t="s">
+      <c r="BP10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="T11" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+    </row>
+    <row r="12" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="X12" s="5" t="s">
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="AC12" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:90" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="Y13" s="5">
+      <c r="Q13" s="6"/>
+      <c r="AD13" s="5">
         <v>6</v>
       </c>
-      <c r="AM13" s="1"/>
-      <c r="AN13" s="10"/>
-      <c r="AP13" s="9">
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="10"/>
+      <c r="AU13" s="9">
         <v>123</v>
       </c>
-      <c r="AQ13" s="9"/>
-      <c r="AR13" s="9"/>
-    </row>
-    <row r="14" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="AV13" s="9"/>
+      <c r="AW13" s="9"/>
+    </row>
+    <row r="14" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="Z14" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="X14" s="5" t="s">
+      <c r="AC14" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="Y14" s="5" t="s">
+      <c r="AD14" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="BL14" s="5" t="s">
+      <c r="BQ14" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="X15" s="5" t="s">
+      <c r="AC15" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="Y15" s="5" t="s">
+      <c r="AD15" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AB15" s="5" t="s">
+      <c r="AG15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="BM15" s="5" t="s">
+      <c r="BR15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BN15" s="5" t="s">
+      <c r="BS15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BO15" s="5" t="s">
+      <c r="BT15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BP15" s="6" t="s">
+      <c r="BU15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:95" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="AM16" s="11" t="s">
+      <c r="AR16" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AN16" s="13" t="s">
+      <c r="AS16" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="AP16" s="5">
+      <c r="AU16" s="5">
         <v>123</v>
       </c>
-      <c r="BM16" s="5" t="s">
+      <c r="BR16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BN16" s="5" t="s">
+      <c r="BS16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BO16" s="6" t="s">
+      <c r="BT16" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="X17" s="5" t="s">
+      <c r="AC17" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="Y17" s="5" t="s">
+      <c r="AD17" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="BP17" s="5" t="s">
+      <c r="BU17" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:91" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="X18" s="5" t="s">
+      <c r="Q18" s="6"/>
+      <c r="AC18" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="Y18" s="5" t="s">
+      <c r="AD18" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="AM18" s="3"/>
-      <c r="AN18" s="10"/>
-      <c r="AP18" s="9">
+      <c r="AR18" s="3"/>
+      <c r="AS18" s="10"/>
+      <c r="AU18" s="9">
         <v>1234</v>
       </c>
-      <c r="AQ18" s="9"/>
-      <c r="AR18" s="9"/>
-    </row>
-    <row r="19" spans="1:91" x14ac:dyDescent="0.35">
+      <c r="AV18" s="9"/>
+      <c r="AW18" s="9"/>
+    </row>
+    <row r="19" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="X19" s="5" t="s">
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="AC19" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="AM19" s="1"/>
-      <c r="AP19" s="5">
+      <c r="AR19" s="1"/>
+      <c r="AU19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="Z20" s="5" t="s">
+      <c r="AE20" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="AH20" s="8"/>
-      <c r="AI20" s="9"/>
-      <c r="AJ20" s="9"/>
-    </row>
-    <row r="21" spans="1:91" x14ac:dyDescent="0.35">
+      <c r="AM20" s="8"/>
+      <c r="AN20" s="9"/>
+      <c r="AO20" s="9"/>
+    </row>
+    <row r="21" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="R21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="S21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="AC21" t="s">
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="AH21" t="s">
         <v>174</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AI21" t="s">
         <v>175</v>
       </c>
-      <c r="AE21" t="s">
+      <c r="AJ21" t="s">
         <v>176</v>
       </c>
-      <c r="AF21" t="s">
+      <c r="AK21" t="s">
         <v>157</v>
       </c>
-      <c r="AG21" t="s">
+      <c r="AL21" t="s">
         <v>157</v>
       </c>
-      <c r="AH21" s="14" t="s">
+      <c r="AM21" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="AI21" s="15" t="s">
+      <c r="AN21" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="AJ21" s="15" t="s">
+      <c r="AO21" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="AK21"/>
-      <c r="AL21"/>
-    </row>
-    <row r="22" spans="1:91" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="AP21"/>
+      <c r="AQ21"/>
+    </row>
+    <row r="22" spans="1:96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>181</v>
       </c>
-      <c r="M22" t="s">
+      <c r="R22" t="s">
         <v>182</v>
       </c>
-      <c r="N22" t="s">
+      <c r="S22" t="s">
         <v>183</v>
       </c>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="AC22" t="s">
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="AH22" t="s">
         <v>35</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AI22" t="s">
         <v>184</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AJ22" t="s">
         <v>185</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AL22" t="s">
         <v>186</v>
       </c>
-      <c r="AH22" t="s">
+      <c r="AM22" t="s">
         <v>187</v>
       </c>
-      <c r="AI22">
+      <c r="AN22">
         <v>9898989898</v>
       </c>
-      <c r="AJ22" s="15" t="s">
+      <c r="AO22" s="15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:91" ht="174" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:96" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="R23" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="S23" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="AC23" s="5" t="s">
+      <c r="AH23" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="AD23" s="5" t="s">
+      <c r="AI23" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="AG23" s="5" t="s">
+      <c r="AL23" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="AH23" s="11" t="s">
+      <c r="AM23" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="AI23" s="11" t="s">
+      <c r="AN23" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="AL23" s="16" t="s">
+      <c r="AQ23" s="16" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:91" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="AQ24" t="s">
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AV24" t="s">
         <v>204</v>
       </c>
-      <c r="AR24" t="s">
+      <c r="AW24" t="s">
         <v>205</v>
       </c>
-      <c r="BQ24" s="5" t="s">
+      <c r="BV24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BR24" s="5" t="s">
+      <c r="BW24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BS24" s="5" t="s">
+      <c r="BX24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BT24" s="5" t="s">
+      <c r="BY24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BU24" s="5" t="s">
+      <c r="BZ24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BV24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BW24" s="5" t="s">
+      <c r="CB24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BX24" s="5">
+      <c r="CC24" s="5">
         <v>9</v>
       </c>
-      <c r="BY24" s="5">
+      <c r="CD24" s="5">
         <v>10</v>
       </c>
-      <c r="BZ24" s="5" t="s">
+      <c r="CE24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="CA24" s="12">
+      <c r="CF24" s="12">
         <v>40000</v>
       </c>
-      <c r="CB24" s="5">
+      <c r="CG24" s="5">
         <v>12</v>
       </c>
-      <c r="CC24" s="12">
+      <c r="CH24" s="12">
         <v>1000000</v>
       </c>
-      <c r="CD24" s="5" t="s">
+      <c r="CI24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="CE24" s="5" t="s">
+      <c r="CJ24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="CF24" s="5">
+      <c r="CK24" s="5">
         <v>57501</v>
       </c>
-      <c r="CG24" s="5" t="s">
+      <c r="CL24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="CH24" s="5" t="s">
+      <c r="CM24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CI24" s="5" t="s">
+      <c r="CN24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CJ24" s="5" t="s">
+      <c r="CO24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="CK24" s="5" t="s">
+      <c r="CP24" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:91" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:96" ht="195" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="L25" s="6"/>
-      <c r="M25" t="s">
+      <c r="Q25" s="6"/>
+      <c r="R25" t="s">
         <v>131</v>
       </c>
-      <c r="N25" s="18" t="s">
+      <c r="S25" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="AC25" t="s">
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="AH25" t="s">
         <v>215</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AI25" t="s">
         <v>216</v>
-      </c>
-      <c r="AE25"/>
-      <c r="AF25"/>
-      <c r="AG25" t="s">
-        <v>217</v>
-      </c>
-      <c r="AH25">
-        <v>19801</v>
-      </c>
-      <c r="AI25">
-        <v>9898989898</v>
       </c>
       <c r="AJ25"/>
       <c r="AK25"/>
-      <c r="AL25" s="16" t="s">
+      <c r="AL25" t="s">
+        <v>217</v>
+      </c>
+      <c r="AM25">
+        <v>19801</v>
+      </c>
+      <c r="AN25">
+        <v>9898989898</v>
+      </c>
+      <c r="AO25"/>
+      <c r="AP25"/>
+      <c r="AQ25" s="16" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:91" x14ac:dyDescent="0.35">
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-    </row>
-    <row r="30" spans="1:91" x14ac:dyDescent="0.35">
-      <c r="CL30" s="5" t="s">
+    <row r="26" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+    </row>
+    <row r="30" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="CQ30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:91" x14ac:dyDescent="0.35">
-      <c r="CL31" s="5" t="s">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="CQ31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:91" x14ac:dyDescent="0.35">
-      <c r="CM32" s="5" t="s">
+    <row r="32" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="CR32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="12:17" x14ac:dyDescent="0.35">
-      <c r="L33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
+    <row r="33" spans="17:22" x14ac:dyDescent="0.25">
       <c r="Q33" s="6"/>
+      <c r="T33" s="6"/>
+      <c r="U33" s="6"/>
+      <c r="V33" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BP15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="J5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="O6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
-    <hyperlink ref="L4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
-    <hyperlink ref="J4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
-    <hyperlink ref="L2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
-    <hyperlink ref="J2" r:id="rId8" xr:uid="{66F73B81-B968-4C82-B793-9099BC4FF784}"/>
-    <hyperlink ref="O2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
-    <hyperlink ref="G8" r:id="rId10" xr:uid="{5BE17100-3B6A-4B64-8895-3FBB3ED3E5B9}"/>
-    <hyperlink ref="O11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
-    <hyperlink ref="K2" r:id="rId12" xr:uid="{14F9C943-C8EA-41B5-B2C0-1606A4BB7DAF}"/>
+    <hyperlink ref="BU15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="O5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
+    <hyperlink ref="T6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
+    <hyperlink ref="T5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
+    <hyperlink ref="Q4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
+    <hyperlink ref="O4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
+    <hyperlink ref="Q2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
+    <hyperlink ref="O2" r:id="rId8" xr:uid="{66F73B81-B968-4C82-B793-9099BC4FF784}"/>
+    <hyperlink ref="T2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
+    <hyperlink ref="K8" r:id="rId10" xr:uid="{5BE17100-3B6A-4B64-8895-3FBB3ED3E5B9}"/>
+    <hyperlink ref="T11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
+    <hyperlink ref="P2" r:id="rId12" xr:uid="{14F9C943-C8EA-41B5-B2C0-1606A4BB7DAF}"/>
     <hyperlink ref="B2" r:id="rId13" xr:uid="{1F6FEAF9-8E7E-47DB-A889-AED537C581F6}"/>
     <hyperlink ref="D2" r:id="rId14" xr:uid="{361190E9-97EB-4336-8DE0-98559A3DB48A}"/>
+    <hyperlink ref="H2" r:id="rId15" xr:uid="{D78A52DD-CB2E-4F8E-9CE9-DFF110C0FD1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HF-Unit Testcase - we are here for you (68) Testcase Commit tetscase, helper, testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA975B7-1201-40C9-A1A8-CE8CC1B070C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9176998F-16E5-412D-9A3C-4A04D7FBFBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="237">
   <si>
     <t>UserName</t>
   </si>
@@ -723,6 +723,30 @@
   <si>
     <t>pro deal form</t>
   </si>
+  <si>
+    <t>SuccessPage</t>
+  </si>
+  <si>
+    <t>Chat live with our service reps,Call our service line. Reach out to us at,Drop us a message to our customer support box</t>
+  </si>
+  <si>
+    <t>tel:1234567890,mailto:support@hydroflask.com</t>
+  </si>
+  <si>
+    <t>bottles-drinkware,kitchenware</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>hyperlink</t>
+  </si>
+  <si>
+    <t>categorylinks</t>
+  </si>
+  <si>
+    <t>2 Day</t>
+  </si>
 </sst>
 </file>
 
@@ -731,7 +755,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -774,8 +798,23 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -786,6 +825,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -802,7 +847,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -833,6 +878,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1114,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR33"/>
+  <dimension ref="A1:CU33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AR4" sqref="AR4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,94 +1183,94 @@
     <col min="6" max="6" width="43.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.7109375" style="5" customWidth="1"/>
-    <col min="11" max="12" width="52.28515625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="67.85546875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="87.140625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.7109375" style="5" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="30.7109375" style="5" customWidth="1"/>
-    <col min="22" max="22" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="29.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30.5703125" style="5" customWidth="1"/>
-    <col min="32" max="32" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19" style="5" customWidth="1"/>
-    <col min="34" max="34" width="19.7109375" style="5" customWidth="1"/>
-    <col min="35" max="35" width="22.28515625" style="5" customWidth="1"/>
-    <col min="36" max="36" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11" style="5" customWidth="1"/>
-    <col min="42" max="42" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9" style="5" customWidth="1"/>
-    <col min="44" max="44" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="97" max="16384" width="56.85546875" style="5"/>
+    <col min="9" max="13" width="30.7109375" style="5" customWidth="1"/>
+    <col min="14" max="15" width="52.28515625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="67.85546875" style="5" customWidth="1"/>
+    <col min="17" max="17" width="87.140625" style="5" customWidth="1"/>
+    <col min="18" max="18" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.7109375" style="5" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="30.7109375" style="5" customWidth="1"/>
+    <col min="25" max="25" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="38" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.5703125" style="5" customWidth="1"/>
+    <col min="35" max="35" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19" style="5" customWidth="1"/>
+    <col min="37" max="37" width="19.7109375" style="5" customWidth="1"/>
+    <col min="38" max="38" width="22.28515625" style="5" customWidth="1"/>
+    <col min="39" max="39" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11" style="5" customWidth="1"/>
+    <col min="45" max="45" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9" style="5" customWidth="1"/>
+    <col min="47" max="47" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="100" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1246,263 +1301,272 @@
       <c r="J1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="BA1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CK1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CL1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CN1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="CL1" s="4" t="s">
+      <c r="CO1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CM1" s="4" t="s">
+      <c r="CP1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CN1" s="4" t="s">
+      <c r="CQ1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CO1" s="4" t="s">
+      <c r="CR1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CP1" s="4" t="s">
+      <c r="CS1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CQ1" s="5" t="s">
+      <c r="CT1" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1525,123 +1589,123 @@
         <v>228</v>
       </c>
       <c r="J2" s="21"/>
-      <c r="O2" s="6" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="R2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
-      <c r="AA2" s="6" t="s">
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
-      <c r="AH2" s="5" t="s">
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="AL2" s="5" t="s">
+      <c r="AO2" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="AM2" s="11" t="s">
+      <c r="AP2" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="AN2" s="5">
+      <c r="AQ2" s="5">
         <v>9898989898</v>
       </c>
-      <c r="AO2" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="AR2" s="11"/>
-      <c r="AS2" s="13"/>
-    </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="AR2" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="13"/>
+    </row>
+    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="5" t="s">
+      <c r="T3" s="6"/>
+      <c r="U3" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="7" t="s">
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
       <c r="AE3" s="6"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
-      <c r="AM3" s="8"/>
-      <c r="AN3" s="9"/>
-      <c r="AO3" s="9"/>
-    </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="9"/>
+      <c r="AR3" s="9"/>
+    </row>
+    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6" t="s">
+      <c r="S4" s="6"/>
+      <c r="T4" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="W4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="U4" s="6"/>
-      <c r="V4" s="5" t="s">
+      <c r="X4" s="6"/>
+      <c r="Y4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="W4" s="7"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
+      <c r="Z4" s="7"/>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
@@ -1649,65 +1713,65 @@
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
-      <c r="AM4" s="8"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
-    </row>
-    <row r="5" spans="1:95" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="9"/>
+    </row>
+    <row r="5" spans="1:98" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="R5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="V5" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="W5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="5" t="s">
+      <c r="X5" s="6"/>
+      <c r="Y5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="10"/>
-      <c r="AU5" s="9">
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="10"/>
+      <c r="AX5" s="9">
         <v>123</v>
       </c>
-      <c r="AV5" s="9"/>
-      <c r="AW5" s="9"/>
-    </row>
-    <row r="6" spans="1:95" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AY5" s="9"/>
+      <c r="AZ5" s="9"/>
+    </row>
+    <row r="6" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="5" t="s">
+      <c r="T6" s="6"/>
+      <c r="U6" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="V6" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="W6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="U6" s="6"/>
-      <c r="V6" s="5" t="s">
+      <c r="X6" s="6"/>
+      <c r="Y6" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
@@ -1716,564 +1780,684 @@
       <c r="AE6" s="6"/>
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
-    </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+    </row>
+    <row r="7" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="Q7" s="6"/>
       <c r="T7" s="6"/>
-      <c r="U7" s="6" t="s">
+      <c r="W7" s="6"/>
+      <c r="X7" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
-    </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+    </row>
+    <row r="8" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="N8" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6" t="s">
+      <c r="O8" s="6"/>
+      <c r="P8" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="Q8" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
-      <c r="AX8" s="5" t="s">
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="BA8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AY8" s="5" t="s">
+      <c r="BB8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AZ8" s="5">
+      <c r="BC8" s="5">
         <v>123456</v>
       </c>
-      <c r="BA8" s="5" t="s">
+      <c r="BD8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="BB8" s="5" t="s">
+      <c r="BE8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="BC8" s="5" t="s">
+      <c r="BF8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>142</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="BD9" s="5" t="s">
+      <c r="BG9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="BE10" s="2" t="s">
+      <c r="BH10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="BF10" s="2" t="s">
+      <c r="BI10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BG10" s="2" t="s">
+      <c r="BJ10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BH10" s="2" t="s">
+      <c r="BK10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="BI10" s="2" t="s">
+      <c r="BL10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BJ10" s="2" t="s">
+      <c r="BM10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BK10" s="2">
+      <c r="BN10" s="2">
         <v>27</v>
       </c>
-      <c r="BL10" s="2" t="s">
+      <c r="BO10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BM10" s="2" t="s">
+      <c r="BP10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BN10" s="2" t="s">
+      <c r="BQ10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BO10" s="2">
+      <c r="BR10" s="2">
         <v>2</v>
       </c>
-      <c r="BP10" s="2" t="s">
+      <c r="BS10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="T11" s="6" t="s">
+      <c r="W11" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
       <c r="X11" s="6"/>
-    </row>
-    <row r="12" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+    </row>
+    <row r="12" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
-      <c r="AC12" s="5" t="s">
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AF12" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="Q13" s="6"/>
-      <c r="AD13" s="5">
+      <c r="T13" s="6"/>
+      <c r="AG13" s="5">
         <v>6</v>
       </c>
-      <c r="AR13" s="1"/>
-      <c r="AS13" s="10"/>
-      <c r="AU13" s="9">
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="10"/>
+      <c r="AX13" s="9">
         <v>123</v>
       </c>
-      <c r="AV13" s="9"/>
-      <c r="AW13" s="9"/>
-    </row>
-    <row r="14" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="AY13" s="9"/>
+      <c r="AZ13" s="9"/>
+    </row>
+    <row r="14" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="Z14" s="5" t="s">
+      <c r="AC14" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="AC14" s="5" t="s">
+      <c r="AF14" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="AD14" s="5" t="s">
+      <c r="AG14" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="BQ14" s="5" t="s">
+      <c r="BT14" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="AC15" s="5" t="s">
+      <c r="AF15" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="AD15" s="5" t="s">
+      <c r="AG15" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AG15" s="5" t="s">
+      <c r="AJ15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="BR15" s="5" t="s">
+      <c r="BU15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BS15" s="5" t="s">
+      <c r="BV15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BT15" s="5" t="s">
+      <c r="BW15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BU15" s="6" t="s">
+      <c r="BX15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:95" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="AR16" s="11" t="s">
+      <c r="AU16" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AS16" s="13" t="s">
+      <c r="AV16" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="AU16" s="5">
+      <c r="AX16" s="5">
         <v>123</v>
       </c>
-      <c r="BR16" s="5" t="s">
+      <c r="BU16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BS16" s="5" t="s">
+      <c r="BV16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BT16" s="6" t="s">
+      <c r="BW16" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="AC17" s="5" t="s">
+      <c r="AF17" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="AD17" s="5" t="s">
+      <c r="AG17" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="BU17" s="5" t="s">
+      <c r="BX17" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="Q18" s="6"/>
-      <c r="AC18" s="5" t="s">
+      <c r="T18" s="6"/>
+      <c r="AF18" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="AD18" s="5" t="s">
+      <c r="AG18" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="AR18" s="3"/>
-      <c r="AS18" s="10"/>
-      <c r="AU18" s="9">
+      <c r="AU18" s="3"/>
+      <c r="AV18" s="10"/>
+      <c r="AX18" s="9">
         <v>1234</v>
       </c>
-      <c r="AV18" s="9"/>
-      <c r="AW18" s="9"/>
-    </row>
-    <row r="19" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="AY18" s="9"/>
+      <c r="AZ18" s="9"/>
+    </row>
+    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
-      <c r="AC19" s="5" t="s">
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AF19" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="AR19" s="1"/>
-      <c r="AU19" s="5">
+      <c r="AU19" s="1"/>
+      <c r="AX19" s="5">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="AE20" s="5" t="s">
+      <c r="AH20" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="AM20" s="8"/>
-      <c r="AN20" s="9"/>
-      <c r="AO20" s="9"/>
-    </row>
-    <row r="21" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="9"/>
+      <c r="AR20" s="9"/>
+    </row>
+    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="R21" s="5" t="s">
+      <c r="U21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="S21" s="5" t="s">
+      <c r="V21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="AH21" t="s">
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="AK21" t="s">
         <v>174</v>
       </c>
-      <c r="AI21" t="s">
+      <c r="AL21" t="s">
         <v>175</v>
       </c>
-      <c r="AJ21" t="s">
+      <c r="AM21" t="s">
         <v>176</v>
       </c>
-      <c r="AK21" t="s">
+      <c r="AN21" t="s">
         <v>157</v>
       </c>
-      <c r="AL21" t="s">
+      <c r="AO21" t="s">
         <v>157</v>
       </c>
-      <c r="AM21" s="14" t="s">
+      <c r="AP21" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="AN21" s="15" t="s">
+      <c r="AQ21" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="AO21" s="15" t="s">
+      <c r="AR21" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="AP21"/>
-      <c r="AQ21"/>
-    </row>
-    <row r="22" spans="1:96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AS21"/>
+      <c r="AT21"/>
+    </row>
+    <row r="22" spans="1:99" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>181</v>
       </c>
-      <c r="R22" t="s">
+      <c r="U22" t="s">
         <v>182</v>
       </c>
-      <c r="S22" t="s">
+      <c r="V22" t="s">
         <v>183</v>
       </c>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
-      <c r="AH22" t="s">
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="AK22" t="s">
         <v>35</v>
       </c>
-      <c r="AI22" t="s">
+      <c r="AL22" t="s">
         <v>184</v>
       </c>
-      <c r="AJ22" t="s">
+      <c r="AM22" t="s">
         <v>185</v>
       </c>
-      <c r="AL22" t="s">
+      <c r="AO22" t="s">
         <v>186</v>
       </c>
-      <c r="AM22" t="s">
+      <c r="AP22" t="s">
         <v>187</v>
       </c>
-      <c r="AN22">
+      <c r="AQ22">
         <v>9898989898</v>
       </c>
-      <c r="AO22" s="15" t="s">
+      <c r="AR22" s="15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:96" ht="180" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:99" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="R23" s="5" t="s">
+      <c r="U23" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="S23" s="5" t="s">
+      <c r="V23" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="AH23" s="5" t="s">
+      <c r="AK23" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="AI23" s="5" t="s">
+      <c r="AL23" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="AL23" s="5" t="s">
+      <c r="AO23" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="AM23" s="11" t="s">
+      <c r="AP23" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="AN23" s="11" t="s">
+      <c r="AQ23" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="AQ23" s="16" t="s">
+      <c r="AT23" s="16" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="AC24" s="6"/>
-      <c r="AV24" t="s">
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AY24" t="s">
         <v>204</v>
       </c>
-      <c r="AW24" t="s">
+      <c r="AZ24" t="s">
         <v>205</v>
       </c>
-      <c r="BV24" s="5" t="s">
+      <c r="BY24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BW24" s="5" t="s">
+      <c r="BZ24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BX24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BY24" s="5" t="s">
+      <c r="CB24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BZ24" s="5" t="s">
+      <c r="CC24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CD24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CE24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="CC24" s="5">
+      <c r="CF24" s="5">
         <v>9</v>
       </c>
-      <c r="CD24" s="5">
+      <c r="CG24" s="5">
         <v>10</v>
       </c>
-      <c r="CE24" s="5" t="s">
+      <c r="CH24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="CF24" s="12">
+      <c r="CI24" s="12">
         <v>40000</v>
       </c>
-      <c r="CG24" s="5">
+      <c r="CJ24" s="5">
         <v>12</v>
       </c>
-      <c r="CH24" s="12">
+      <c r="CK24" s="12">
         <v>1000000</v>
       </c>
-      <c r="CI24" s="5" t="s">
+      <c r="CL24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="CJ24" s="5" t="s">
+      <c r="CM24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="CK24" s="5">
+      <c r="CN24" s="5">
         <v>57501</v>
       </c>
-      <c r="CL24" s="5" t="s">
+      <c r="CO24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="CM24" s="5" t="s">
+      <c r="CP24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CN24" s="5" t="s">
+      <c r="CQ24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CO24" s="5" t="s">
+      <c r="CR24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="CP24" s="5" t="s">
+      <c r="CS24" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:96" ht="195" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:99" ht="195" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="Q25" s="6"/>
-      <c r="R25" t="s">
+      <c r="T25" s="6"/>
+      <c r="U25" t="s">
         <v>131</v>
       </c>
-      <c r="S25" s="18" t="s">
+      <c r="V25" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
-      <c r="AH25" t="s">
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AK25" t="s">
         <v>215</v>
       </c>
-      <c r="AI25" t="s">
+      <c r="AL25" t="s">
         <v>216</v>
       </c>
-      <c r="AJ25"/>
-      <c r="AK25"/>
-      <c r="AL25" t="s">
+      <c r="AM25"/>
+      <c r="AN25"/>
+      <c r="AO25" t="s">
         <v>217</v>
       </c>
-      <c r="AM25">
+      <c r="AP25">
         <v>19801</v>
       </c>
-      <c r="AN25">
+      <c r="AQ25">
         <v>9898989898</v>
       </c>
-      <c r="AO25"/>
-      <c r="AP25"/>
-      <c r="AQ25" s="16" t="s">
+      <c r="AR25"/>
+      <c r="AS25"/>
+      <c r="AT25" s="16" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="O26" s="5" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="O27" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-    </row>
-    <row r="30" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="CQ30" s="5" t="s">
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+    </row>
+    <row r="28" spans="1:99" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="L28" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="M28" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="N28" s="22"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="25"/>
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22"/>
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="22"/>
+      <c r="AH28" s="22"/>
+      <c r="AI28" s="22"/>
+      <c r="AJ28" s="22"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="22"/>
+      <c r="AM28" s="22"/>
+      <c r="AN28" s="22"/>
+      <c r="AO28" s="22"/>
+      <c r="AP28" s="22"/>
+      <c r="AQ28" s="22"/>
+      <c r="AR28" s="22"/>
+      <c r="AS28" s="22"/>
+      <c r="AT28" s="22"/>
+      <c r="AU28" s="22"/>
+      <c r="AV28" s="27"/>
+      <c r="AW28" s="27"/>
+      <c r="AX28" s="22"/>
+      <c r="AY28" s="22"/>
+      <c r="AZ28" s="22"/>
+      <c r="BA28" s="22"/>
+      <c r="BB28" s="22"/>
+      <c r="BC28" s="22"/>
+      <c r="BD28" s="22"/>
+      <c r="BE28" s="22"/>
+      <c r="BF28" s="22"/>
+      <c r="BG28" s="22"/>
+      <c r="BH28" s="22"/>
+      <c r="BI28" s="22"/>
+      <c r="BJ28" s="22"/>
+      <c r="BK28" s="22"/>
+      <c r="BL28" s="27"/>
+      <c r="BM28" s="27"/>
+      <c r="BN28" s="22"/>
+      <c r="BO28" s="22"/>
+      <c r="BP28" s="22"/>
+      <c r="BQ28" s="22"/>
+      <c r="BR28" s="22"/>
+      <c r="BS28" s="22"/>
+      <c r="BT28" s="22"/>
+      <c r="BU28" s="22"/>
+      <c r="BV28" s="22"/>
+      <c r="BW28" s="22"/>
+      <c r="BX28" s="22"/>
+      <c r="BY28" s="22"/>
+      <c r="BZ28" s="22"/>
+      <c r="CA28" s="27"/>
+      <c r="CB28" s="27"/>
+      <c r="CC28" s="22"/>
+      <c r="CD28" s="27"/>
+      <c r="CE28" s="27"/>
+      <c r="CF28" s="22"/>
+      <c r="CG28" s="22"/>
+      <c r="CH28" s="22"/>
+      <c r="CI28" s="22"/>
+      <c r="CJ28" s="22"/>
+      <c r="CK28" s="27"/>
+      <c r="CL28" s="27"/>
+      <c r="CM28" s="22"/>
+      <c r="CN28" s="22"/>
+      <c r="CO28" s="22"/>
+      <c r="CP28" s="27"/>
+      <c r="CQ28" s="27"/>
+      <c r="CR28" s="22"/>
+      <c r="CS28" s="22"/>
+      <c r="CT28" s="22"/>
+    </row>
+    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="CT30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="CQ31" s="5" t="s">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="CT31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="CR32" s="5" t="s">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="CU32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="17:22" x14ac:dyDescent="0.25">
-      <c r="Q33" s="6"/>
+    <row r="33" spans="20:25" x14ac:dyDescent="0.25">
       <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+      <c r="Y33" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="CP28:CQ28"/>
+    <mergeCell ref="AV28:AW28"/>
+    <mergeCell ref="BL28:BM28"/>
+    <mergeCell ref="CA28:CB28"/>
+    <mergeCell ref="CD28:CE28"/>
+    <mergeCell ref="CK28:CL28"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="BU15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="O5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="T6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
-    <hyperlink ref="T5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
-    <hyperlink ref="Q4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
-    <hyperlink ref="O4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
-    <hyperlink ref="Q2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
-    <hyperlink ref="O2" r:id="rId8" xr:uid="{66F73B81-B968-4C82-B793-9099BC4FF784}"/>
-    <hyperlink ref="T2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
-    <hyperlink ref="K8" r:id="rId10" xr:uid="{5BE17100-3B6A-4B64-8895-3FBB3ED3E5B9}"/>
-    <hyperlink ref="T11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
-    <hyperlink ref="P2" r:id="rId12" xr:uid="{14F9C943-C8EA-41B5-B2C0-1606A4BB7DAF}"/>
+    <hyperlink ref="BX15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="R5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
+    <hyperlink ref="W6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
+    <hyperlink ref="W5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
+    <hyperlink ref="T4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
+    <hyperlink ref="R4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
+    <hyperlink ref="T2" r:id="rId7" xr:uid="{5FF8E9F0-2E71-4894-8AF1-C621CCE0D91A}"/>
+    <hyperlink ref="R2" r:id="rId8" xr:uid="{66F73B81-B968-4C82-B793-9099BC4FF784}"/>
+    <hyperlink ref="W2" r:id="rId9" xr:uid="{2E9978F8-526E-43DA-8810-9347FCCE65FA}"/>
+    <hyperlink ref="N8" r:id="rId10" xr:uid="{5BE17100-3B6A-4B64-8895-3FBB3ED3E5B9}"/>
+    <hyperlink ref="W11" r:id="rId11" xr:uid="{449D881A-BD5A-4CAB-AEC9-6420F45023CE}"/>
+    <hyperlink ref="S2" r:id="rId12" xr:uid="{14F9C943-C8EA-41B5-B2C0-1606A4BB7DAF}"/>
     <hyperlink ref="B2" r:id="rId13" xr:uid="{1F6FEAF9-8E7E-47DB-A889-AED537C581F6}"/>
     <hyperlink ref="D2" r:id="rId14" xr:uid="{361190E9-97EB-4336-8DE0-98559A3DB48A}"/>
     <hyperlink ref="H2" r:id="rId15" xr:uid="{D78A52DD-CB2E-4F8E-9CE9-DFF110C0FD1B}"/>
+    <hyperlink ref="L28" r:id="rId16" xr:uid="{95EF516E-7A33-40FC-9785-E5BB382BCD4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Payment page validation test case for Hydroflask and OXO
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{9176998F-16E5-412D-9A3C-4A04D7FBFBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23993F41-1C89-4321-A86E-C73BBDB9A2FC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5E4D3D-D96C-4FF4-9875-9D9E61332C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="248">
   <si>
     <t>UserName</t>
   </si>
@@ -773,6 +773,12 @@
   </si>
   <si>
     <t>Minimum length of this field must be equal or greater than 8 symbols. Leading and trailing spaces will be ignored.</t>
+  </si>
+  <si>
+    <t>Order Summary</t>
+  </si>
+  <si>
+    <t>OrderSummaryProduct</t>
   </si>
 </sst>
 </file>
@@ -880,7 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -922,6 +928,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1205,106 +1212,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CZ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" topLeftCell="CY27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CY36" sqref="CY36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="20.7265625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.54296875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="43.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="30.7265625" style="5" customWidth="1"/>
-    <col min="14" max="15" width="52.26953125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="67.81640625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="87.1796875" style="5" customWidth="1"/>
-    <col min="18" max="18" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="30.7265625" style="5" customWidth="1"/>
-    <col min="22" max="22" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="29" width="30.7265625" style="5" customWidth="1"/>
-    <col min="30" max="30" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="43.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="30.7109375" style="5" customWidth="1"/>
+    <col min="14" max="15" width="52.28515625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="67.85546875" style="5" customWidth="1"/>
+    <col min="17" max="17" width="87.140625" style="5" customWidth="1"/>
+    <col min="18" max="18" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="30.7109375" style="5" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="29" width="30.7109375" style="5" customWidth="1"/>
+    <col min="30" max="30" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="31.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="30.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="30.54296875" style="5" customWidth="1"/>
+    <col min="33" max="33" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="30.5703125" style="5" customWidth="1"/>
     <col min="40" max="40" width="19" style="5" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="19" style="5" customWidth="1"/>
-    <col min="42" max="42" width="19.7265625" style="5" customWidth="1"/>
-    <col min="43" max="43" width="22.26953125" style="5" customWidth="1"/>
+    <col min="42" max="42" width="19.7109375" style="5" customWidth="1"/>
+    <col min="43" max="43" width="22.28515625" style="5" customWidth="1"/>
     <col min="44" max="44" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="11" style="5" customWidth="1"/>
     <col min="50" max="50" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="9" style="5" customWidth="1"/>
-    <col min="52" max="52" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="19.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="17.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="105" max="16384" width="56.81640625" style="5"/>
+    <col min="102" max="102" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="105" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1614,8 +1621,11 @@
       <c r="CY1" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.35">
+      <c r="CZ1" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1702,7 +1712,7 @@
       <c r="AZ2" s="11"/>
       <c r="BA2" s="13"/>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
@@ -1738,7 +1748,7 @@
       <c r="AV3" s="9"/>
       <c r="AW3" s="9"/>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
@@ -1782,7 +1792,7 @@
       <c r="AV4" s="9"/>
       <c r="AW4" s="9"/>
     </row>
-    <row r="5" spans="1:103" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:104" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>122</v>
       </c>
@@ -1831,7 +1841,7 @@
       <c r="BD5" s="9"/>
       <c r="BE5" s="9"/>
     </row>
-    <row r="6" spans="1:103" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:104" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>123</v>
       </c>
@@ -1864,7 +1874,7 @@
       <c r="AN6" s="6"/>
       <c r="AO6" s="6"/>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>126</v>
       </c>
@@ -1883,7 +1893,7 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="6"/>
     </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>129</v>
       </c>
@@ -1924,7 +1934,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>142</v>
       </c>
@@ -1935,7 +1945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:103" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:104" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>144</v>
       </c>
@@ -1979,7 +1989,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>145</v>
       </c>
@@ -1994,7 +2004,7 @@
       <c r="AE11" s="6"/>
       <c r="AF11" s="6"/>
     </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>149</v>
       </c>
@@ -2010,7 +2020,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:103" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>150</v>
       </c>
@@ -2026,7 +2036,7 @@
       <c r="BD13" s="9"/>
       <c r="BE13" s="9"/>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>151</v>
       </c>
@@ -2043,7 +2053,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>154</v>
       </c>
@@ -2069,7 +2079,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>158</v>
       </c>
@@ -2092,7 +2102,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>161</v>
       </c>
@@ -2106,7 +2116,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:104" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>163</v>
       </c>
@@ -2125,7 +2135,7 @@
       <c r="BD18" s="9"/>
       <c r="BE18" s="9"/>
     </row>
-    <row r="19" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>164</v>
       </c>
@@ -2145,7 +2155,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>169</v>
       </c>
@@ -2156,7 +2166,7 @@
       <c r="AV20" s="9"/>
       <c r="AW20" s="9"/>
     </row>
-    <row r="21" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>173</v>
       </c>
@@ -2199,7 +2209,7 @@
       <c r="AX21"/>
       <c r="AY21"/>
     </row>
-    <row r="22" spans="1:104" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:104" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>181</v>
       </c>
@@ -2237,7 +2247,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:104" ht="174" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:104" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>194</v>
       </c>
@@ -2266,7 +2276,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>203</v>
       </c>
@@ -2347,7 +2357,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:104" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:104" ht="195" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>214</v>
       </c>
@@ -2389,7 +2399,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>219</v>
       </c>
@@ -2397,7 +2407,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>220</v>
       </c>
@@ -2411,7 +2421,7 @@
       <c r="AC27" s="6"/>
       <c r="AD27" s="6"/>
     </row>
-    <row r="28" spans="1:104" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:104" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>229</v>
       </c>
@@ -2472,8 +2482,8 @@
       <c r="AX28" s="22"/>
       <c r="AY28" s="22"/>
       <c r="AZ28" s="22"/>
-      <c r="BA28" s="27"/>
-      <c r="BB28" s="27"/>
+      <c r="BA28" s="29"/>
+      <c r="BB28" s="29"/>
       <c r="BC28" s="22"/>
       <c r="BD28" s="22"/>
       <c r="BE28" s="22"/>
@@ -2488,8 +2498,8 @@
       <c r="BN28" s="22"/>
       <c r="BO28" s="22"/>
       <c r="BP28" s="22"/>
-      <c r="BQ28" s="27"/>
-      <c r="BR28" s="27"/>
+      <c r="BQ28" s="29"/>
+      <c r="BR28" s="29"/>
       <c r="BS28" s="22"/>
       <c r="BT28" s="22"/>
       <c r="BU28" s="22"/>
@@ -2503,43 +2513,51 @@
       <c r="CC28" s="22"/>
       <c r="CD28" s="22"/>
       <c r="CE28" s="22"/>
-      <c r="CF28" s="27"/>
-      <c r="CG28" s="27"/>
+      <c r="CF28" s="29"/>
+      <c r="CG28" s="29"/>
       <c r="CH28" s="22"/>
-      <c r="CI28" s="27"/>
-      <c r="CJ28" s="27"/>
+      <c r="CI28" s="29"/>
+      <c r="CJ28" s="29"/>
       <c r="CK28" s="22"/>
       <c r="CL28" s="22"/>
       <c r="CM28" s="22"/>
       <c r="CN28" s="22"/>
       <c r="CO28" s="22"/>
-      <c r="CP28" s="27"/>
-      <c r="CQ28" s="27"/>
+      <c r="CP28" s="29"/>
+      <c r="CQ28" s="29"/>
       <c r="CR28" s="22"/>
       <c r="CS28" s="22"/>
       <c r="CT28" s="22"/>
-      <c r="CU28" s="27"/>
-      <c r="CV28" s="27"/>
+      <c r="CU28" s="29"/>
+      <c r="CV28" s="29"/>
       <c r="CW28" s="22"/>
       <c r="CX28" s="22"/>
       <c r="CY28" s="22"/>
     </row>
-    <row r="30" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="CY29" s="27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:104" x14ac:dyDescent="0.25">
       <c r="CY30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:104" x14ac:dyDescent="0.25">
       <c r="CY31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:104" x14ac:dyDescent="0.25">
       <c r="CZ32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="22:30" x14ac:dyDescent="0.35">
+    <row r="33" spans="22:30" x14ac:dyDescent="0.25">
       <c r="V33" s="6"/>
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>

</xml_diff>